<commit_message>
Not too sure what has changed, but am sure something has
</commit_message>
<xml_diff>
--- a/pcb/3YP_PARTS_LIST.xlsx
+++ b/pcb/3YP_PARTS_LIST.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Samue\Documents\work\pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E3CC24-3553-4ABA-B5AB-B1AB8AE5DFDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4277D1-FE48-436B-8923-D38DD9337F39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3BF32B11-E6A7-4DC9-B128-7A92B7481BEB}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="109">
   <si>
     <t>PART</t>
   </si>
@@ -281,9 +281,6 @@
     <t>C1</t>
   </si>
   <si>
-    <t>C2, C4, C6</t>
-  </si>
-  <si>
     <t>C3, C5</t>
   </si>
   <si>
@@ -348,6 +345,21 @@
   </si>
   <si>
     <t>With VAT</t>
+  </si>
+  <si>
+    <t>SI7006-A20-IM1R</t>
+  </si>
+  <si>
+    <t>Low Power Temp/Humidity Sensor I2C</t>
+  </si>
+  <si>
+    <t>https://onecall.farnell.com/silicon-labs/si7006-a20-im1r/humidity-temp-sensor-dfn-6/dp/3105971</t>
+  </si>
+  <si>
+    <t>HM1</t>
+  </si>
+  <si>
+    <t>C2, C4, C6, C7</t>
   </si>
 </sst>
 </file>
@@ -791,7 +803,7 @@
   <dimension ref="A1:S59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,19 +846,19 @@
         <v>13</v>
       </c>
       <c r="I1" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="J1" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="J1" s="7" t="s">
-        <v>87</v>
-      </c>
       <c r="K1" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L1" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="M1" s="7" t="s">
         <v>90</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1195,7 +1207,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="B10" s="12">
         <v>9</v>
@@ -1204,7 +1216,7 @@
         <v>45</v>
       </c>
       <c r="D10" s="12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>5</v>
@@ -1226,14 +1238,14 @@
       </c>
       <c r="K10" s="3">
         <f>D10*K24</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="L10" s="3">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="M10" s="19">
         <f t="shared" si="0"/>
-        <v>3.5100000000000002</v>
+        <v>4.6800000000000006</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -1281,7 +1293,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B12" s="12">
         <v>11</v>
@@ -1502,7 +1514,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D17" s="12">
         <v>1</v>
@@ -1539,7 +1551,7 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B18" s="12">
         <v>17</v>
@@ -1554,13 +1566,13 @@
         <v>12</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G18" s="12" t="s">
         <v>70</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I18" s="18">
         <v>0.33200000000000002</v>
@@ -1582,7 +1594,7 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B19" s="12">
         <v>18</v>
@@ -1625,7 +1637,7 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B20" s="12">
         <v>19</v>
@@ -1674,13 +1686,13 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B21" s="12">
         <v>20</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D21" s="12">
         <v>1</v>
@@ -1692,10 +1704,10 @@
         <v>2856691</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I21" s="18">
         <v>0.23</v>
@@ -1717,13 +1729,13 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B22" s="12">
         <v>21</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D22" s="12">
         <v>1</v>
@@ -1735,10 +1747,10 @@
         <v>2909992</v>
       </c>
       <c r="G22" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="H22" s="17" t="s">
         <v>100</v>
-      </c>
-      <c r="H22" s="17" t="s">
-        <v>101</v>
       </c>
       <c r="I22" s="18">
         <v>2.1800000000000002</v>
@@ -1759,19 +1771,45 @@
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="10"/>
+      <c r="A23" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B23" s="12">
+        <v>22</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>105</v>
+      </c>
       <c r="D23" s="12">
-        <f>SUM(D2:D22)</f>
-        <v>33</v>
-      </c>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="M23" s="20">
-        <f>SUM(M2:M22)</f>
-        <v>98.293199999999999</v>
+        <v>1</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" s="12">
+        <v>3105971</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="I23" s="18">
+        <v>2.44</v>
+      </c>
+      <c r="J23" s="12">
+        <v>1</v>
+      </c>
+      <c r="K23" s="3">
+        <v>4</v>
+      </c>
+      <c r="L23" s="3">
+        <v>4</v>
+      </c>
+      <c r="M23" s="19">
+        <f>L23*I23</f>
+        <v>9.76</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
@@ -1783,10 +1821,14 @@
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
       <c r="J24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K24">
         <v>4</v>
+      </c>
+      <c r="M24" s="20">
+        <f>SUM(M2:M23)</f>
+        <v>109.22320000000001</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
@@ -1807,20 +1849,18 @@
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
       <c r="L26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M26" s="20">
-        <f>1.2*M23</f>
-        <v>117.95183999999999</v>
+        <f>1.2*M24</f>
+        <v>131.06783999999999</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="B27" s="12"/>
       <c r="C27" s="10"/>
-      <c r="D27" s="12">
-        <v>6</v>
-      </c>
+      <c r="D27" s="12"/>
       <c r="E27" s="12"/>
       <c r="G27" s="12"/>
     </row>
@@ -1828,9 +1868,7 @@
       <c r="A28" s="10"/>
       <c r="B28" s="12"/>
       <c r="C28" s="10"/>
-      <c r="D28" s="12">
-        <v>5</v>
-      </c>
+      <c r="D28" s="12"/>
       <c r="E28" s="12"/>
       <c r="G28" s="12"/>
     </row>
@@ -1838,9 +1876,7 @@
       <c r="A29" s="10"/>
       <c r="B29" s="12"/>
       <c r="C29" s="10"/>
-      <c r="D29" s="12">
-        <v>9</v>
-      </c>
+      <c r="D29" s="12"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
       <c r="G29" s="12"/>
@@ -1850,9 +1886,7 @@
       <c r="A30" s="10"/>
       <c r="B30" s="12"/>
       <c r="C30" s="10"/>
-      <c r="D30" s="12">
-        <v>13</v>
-      </c>
+      <c r="D30" s="12"/>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
@@ -1862,10 +1896,7 @@
       <c r="A31" s="10"/>
       <c r="B31" s="12"/>
       <c r="C31" s="10"/>
-      <c r="D31" s="12">
-        <f>SUM(D27:D30)</f>
-        <v>33</v>
-      </c>
+      <c r="D31" s="12"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
       <c r="G31" s="12"/>
@@ -2163,8 +2194,9 @@
     <hyperlink ref="H18" r:id="rId19" xr:uid="{E6EFD2F6-36C3-407C-9BA4-06F23821F1B5}"/>
     <hyperlink ref="H21" r:id="rId20" xr:uid="{7C225CFB-088D-4C0E-9F94-BF82F6D07FB6}"/>
     <hyperlink ref="H22" r:id="rId21" xr:uid="{DD603BB5-BEA7-476C-9FC5-3BB769AB8A18}"/>
+    <hyperlink ref="H23" r:id="rId22" xr:uid="{816AB84F-C82D-403C-8336-D31E050AB85D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId22"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ordering parts. Crossed some off
</commit_message>
<xml_diff>
--- a/pcb/3YP_PARTS_LIST.xlsx
+++ b/pcb/3YP_PARTS_LIST.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Users\Sam\Work\3yp git\3YP\pcb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Samue\Documents\work\pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7FDAD97-69CA-4DB2-ABC1-822ED79743EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-40875" yWindow="6105" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="111">
   <si>
     <t>PART</t>
   </si>
@@ -359,16 +360,23 @@
   </si>
   <si>
     <t>C2, C6, C7, C9, C10</t>
+  </si>
+  <si>
+    <t>Done?</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -410,6 +418,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -428,12 +443,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -483,14 +499,32 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00FF00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -798,11 +832,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,7 +853,7 @@
     <col min="11" max="11" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>10</v>
       </c>
@@ -859,8 +893,14 @@
       <c r="M1" s="7" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N1" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>9</v>
       </c>
@@ -893,16 +933,23 @@
       </c>
       <c r="K2" s="3">
         <f>D2*J28</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L2" s="3">
         <v>4</v>
       </c>
-      <c r="M2" s="19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M2" s="19">
+        <v>0</v>
+      </c>
+      <c r="N2" s="21">
+        <f>M2*1.2</f>
+        <v>0</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>22</v>
       </c>
@@ -928,24 +975,31 @@
         <v>18</v>
       </c>
       <c r="I3" s="18">
-        <v>0.19</v>
+        <v>0.192</v>
       </c>
       <c r="J3" s="12">
         <v>10</v>
       </c>
       <c r="K3" s="3">
         <f>D3*J28</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="L3" s="3">
         <v>10</v>
       </c>
       <c r="M3" s="19">
         <f t="shared" ref="M3:M20" si="0">L3*I3</f>
-        <v>1.9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1.92</v>
+      </c>
+      <c r="N3" s="21">
+        <f t="shared" ref="N3:N24" si="1">M3*1.2</f>
+        <v>2.3039999999999998</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>23</v>
       </c>
@@ -978,7 +1032,7 @@
       </c>
       <c r="K4" s="3">
         <f>D4*J28</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L4" s="3">
         <v>5</v>
@@ -987,8 +1041,15 @@
         <f t="shared" si="0"/>
         <v>0.63</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4" s="21">
+        <f t="shared" si="1"/>
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>27</v>
       </c>
@@ -1021,17 +1082,24 @@
       </c>
       <c r="K5" s="3">
         <f>D5*J28</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L5" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M5" s="19">
         <f t="shared" si="0"/>
-        <v>19.72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <v>24.65</v>
+      </c>
+      <c r="N5" s="21">
+        <f t="shared" si="1"/>
+        <v>29.58</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>32</v>
       </c>
@@ -1064,7 +1132,7 @@
       </c>
       <c r="K6" s="3">
         <f>D6*J28</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L6" s="3">
         <v>4</v>
@@ -1073,8 +1141,13 @@
         <f t="shared" si="0"/>
         <v>22.68</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6" s="21">
+        <f t="shared" si="1"/>
+        <v>27.215999999999998</v>
+      </c>
+      <c r="O6" s="3"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>35</v>
       </c>
@@ -1107,7 +1180,7 @@
       </c>
       <c r="K7" s="3">
         <f>D7*J28</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L7" s="3">
         <v>4</v>
@@ -1116,8 +1189,15 @@
         <f t="shared" si="0"/>
         <v>9.9600000000000009</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7" s="21">
+        <f t="shared" si="1"/>
+        <v>11.952</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>40</v>
       </c>
@@ -1150,17 +1230,24 @@
       </c>
       <c r="K8" s="3">
         <f>D8*J28</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L8" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M8" s="19">
         <f t="shared" si="0"/>
-        <v>14.12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>17.649999999999999</v>
+      </c>
+      <c r="N8" s="21">
+        <f t="shared" si="1"/>
+        <v>21.179999999999996</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>107</v>
       </c>
@@ -1193,17 +1280,24 @@
       </c>
       <c r="K9" s="3">
         <f>D9*J28</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="L9" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="M9" s="19">
         <f t="shared" si="0"/>
-        <v>2.9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+        <v>5.8</v>
+      </c>
+      <c r="N9" s="21">
+        <f t="shared" si="1"/>
+        <v>6.96</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>108</v>
       </c>
@@ -1236,17 +1330,23 @@
       </c>
       <c r="K10" s="3">
         <f>D10*J28</f>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="L10" s="3">
         <v>20</v>
       </c>
       <c r="M10" s="19">
-        <f t="shared" si="0"/>
-        <v>4.6800000000000006</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="N10" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>44</v>
       </c>
@@ -1279,17 +1379,24 @@
       </c>
       <c r="K11" s="3">
         <f>D11*J28</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L11" s="3">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="M11" s="19">
         <f t="shared" si="0"/>
+        <v>0.47100000000000003</v>
+      </c>
+      <c r="N11" s="21">
+        <f t="shared" si="1"/>
         <v>0.56520000000000004</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O11" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>89</v>
       </c>
@@ -1322,17 +1429,23 @@
       </c>
       <c r="K12" s="3">
         <f>D12*J28</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="L12" s="3">
         <v>10</v>
       </c>
       <c r="M12" s="19">
-        <f t="shared" si="0"/>
-        <v>2.8100000000000005</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="N12" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>74</v>
       </c>
@@ -1365,17 +1478,23 @@
       </c>
       <c r="K13" s="3">
         <f>D13*J28</f>
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="L13" s="3">
         <v>30</v>
       </c>
       <c r="M13" s="19">
-        <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="N13" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>75</v>
       </c>
@@ -1408,17 +1527,23 @@
       </c>
       <c r="K14" s="3">
         <f>D14*J28</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="L14" s="3">
         <v>10</v>
       </c>
       <c r="M14" s="19">
-        <f t="shared" si="0"/>
-        <v>0.20600000000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="N14" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>76</v>
       </c>
@@ -1451,17 +1576,23 @@
       </c>
       <c r="K15" s="3">
         <f>D15*J28</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L15" s="3">
         <v>10</v>
       </c>
       <c r="M15" s="19">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="N15" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>77</v>
       </c>
@@ -1494,14 +1625,20 @@
       </c>
       <c r="K16" s="3">
         <f>D16*J28</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="L16" s="3">
         <v>10</v>
       </c>
       <c r="M16" s="19">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0</v>
+      </c>
+      <c r="N16" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
@@ -1537,7 +1674,7 @@
       </c>
       <c r="K17" s="3">
         <f>D17*J28</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L17" s="3">
         <v>10</v>
@@ -1546,6 +1683,13 @@
         <f t="shared" si="0"/>
         <v>2.6</v>
       </c>
+      <c r="N17" s="21">
+        <f t="shared" si="1"/>
+        <v>3.12</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
@@ -1580,7 +1724,7 @@
       </c>
       <c r="K18" s="3">
         <f>D18*J28</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L18" s="3">
         <v>25</v>
@@ -1589,6 +1733,11 @@
         <f t="shared" si="0"/>
         <v>8.75</v>
       </c>
+      <c r="N18" s="21">
+        <f t="shared" si="1"/>
+        <v>10.5</v>
+      </c>
+      <c r="O18" s="3"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
@@ -1623,14 +1772,21 @@
       </c>
       <c r="K19" s="3">
         <f>D19*J28</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L19" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M19" s="19">
         <f t="shared" si="0"/>
-        <v>2.7440000000000002</v>
+        <v>3.43</v>
+      </c>
+      <c r="N19" s="21">
+        <f t="shared" si="1"/>
+        <v>4.1159999999999997</v>
+      </c>
+      <c r="O19" s="3" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
@@ -1666,7 +1822,7 @@
       </c>
       <c r="K20" s="3">
         <f>D20*J28</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="L20" s="3">
         <v>15</v>
@@ -1675,8 +1831,13 @@
         <f t="shared" si="0"/>
         <v>2.7749999999999999</v>
       </c>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
+      <c r="N20" s="21">
+        <f t="shared" si="1"/>
+        <v>3.3299999999999996</v>
+      </c>
+      <c r="O20" s="3" t="s">
+        <v>110</v>
+      </c>
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
@@ -1715,7 +1876,7 @@
       </c>
       <c r="K21" s="3">
         <f>D21*J28</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L21" s="3">
         <v>10</v>
@@ -1724,6 +1885,13 @@
         <f>L21*I21</f>
         <v>2.3000000000000003</v>
       </c>
+      <c r="N21" s="21">
+        <f t="shared" si="1"/>
+        <v>2.7600000000000002</v>
+      </c>
+      <c r="O21" s="3" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
@@ -1758,14 +1926,21 @@
       </c>
       <c r="K22" s="3">
         <f>J22*J28</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L22" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M22" s="19">
         <f>L22*I22</f>
-        <v>0</v>
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="N22" s="21">
+        <f t="shared" si="1"/>
+        <v>2.6160000000000001</v>
+      </c>
+      <c r="O22" s="3" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
@@ -1801,14 +1976,21 @@
       </c>
       <c r="K23" s="3">
         <f>J23*J28</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L23" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M23" s="20">
         <f>L23*I23</f>
-        <v>9.76</v>
+        <v>12.2</v>
+      </c>
+      <c r="N23" s="21">
+        <f t="shared" si="1"/>
+        <v>14.639999999999999</v>
+      </c>
+      <c r="O23" s="3" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
@@ -1821,7 +2003,11 @@
       <c r="G24" s="12"/>
       <c r="M24" s="20">
         <f>SUM(M2:M23)</f>
-        <v>110.10020000000003</v>
+        <v>117.99600000000001</v>
+      </c>
+      <c r="N24" s="21">
+        <f t="shared" si="1"/>
+        <v>141.59520000000001</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
@@ -1844,13 +2030,7 @@
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
-      <c r="L26" t="s">
-        <v>95</v>
-      </c>
-      <c r="M26" s="20">
-        <f>1.2*M24</f>
-        <v>132.12024000000002</v>
-      </c>
+      <c r="M26" s="20"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
@@ -1871,7 +2051,11 @@
         <v>106</v>
       </c>
       <c r="J28">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="N28" s="22">
+        <f>N24-N18-N6</f>
+        <v>103.87920000000001</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
@@ -1883,6 +2067,14 @@
       <c r="F29" s="12"/>
       <c r="G29" s="12"/>
       <c r="H29" s="9"/>
+      <c r="L29">
+        <f>SUM(L23,L21,L20,L19,L17,L11,L9,L8,L6,L5,L4,L3)</f>
+        <v>94</v>
+      </c>
+      <c r="N29" s="22">
+        <f>N24-N28</f>
+        <v>37.715999999999994</v>
+      </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="10"/>
@@ -2174,29 +2366,36 @@
       <c r="H59" s="2"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="O2:O23">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
-    <hyperlink ref="H3" r:id="rId2"/>
-    <hyperlink ref="H4" r:id="rId3"/>
-    <hyperlink ref="H5" r:id="rId4"/>
-    <hyperlink ref="H6" r:id="rId5"/>
-    <hyperlink ref="H8" r:id="rId6"/>
-    <hyperlink ref="H7" r:id="rId7"/>
-    <hyperlink ref="H10" r:id="rId8"/>
-    <hyperlink ref="H12" r:id="rId9"/>
-    <hyperlink ref="H11" r:id="rId10"/>
-    <hyperlink ref="H13" r:id="rId11"/>
-    <hyperlink ref="H16" r:id="rId12"/>
-    <hyperlink ref="H15" r:id="rId13"/>
-    <hyperlink ref="H14" r:id="rId14"/>
-    <hyperlink ref="H17" r:id="rId15"/>
-    <hyperlink ref="H19" r:id="rId16"/>
-    <hyperlink ref="H20" r:id="rId17"/>
-    <hyperlink ref="H21" r:id="rId18"/>
-    <hyperlink ref="H22" r:id="rId19"/>
-    <hyperlink ref="H23" r:id="rId20"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="H4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="H5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="H6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="H8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="H7" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="H10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="H12" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="H11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="H13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="H16" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="H15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="H14" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="H17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="H19" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="H20" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="H21" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="H22" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="H23" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="H18" r:id="rId21" xr:uid="{B2D838FA-5C57-4FC8-B5CD-90352BD7ADDE}"/>
+    <hyperlink ref="H9" r:id="rId22" xr:uid="{FC047744-6697-401C-8D39-1AEC0EC47B63}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId21"/>
+  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New board revision 3A
</commit_message>
<xml_diff>
--- a/pcb/3YP_PARTS_LIST.xlsx
+++ b/pcb/3YP_PARTS_LIST.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="REV 2B" sheetId="1" r:id="rId1"/>
+    <sheet name="REV 3A" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="147">
   <si>
     <t>PART</t>
   </si>
@@ -377,6 +378,102 @@
   </si>
   <si>
     <t>Per board:</t>
+  </si>
+  <si>
+    <t>PACKAGE TYPE</t>
+  </si>
+  <si>
+    <t>https://uk.rs-online.com/web/p/temperature-sensors-humidity-sensors/1330170/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDC1080DMBT </t>
+  </si>
+  <si>
+    <t>133-0170</t>
+  </si>
+  <si>
+    <t>WSON</t>
+  </si>
+  <si>
+    <t>J3, J4, J5, J6</t>
+  </si>
+  <si>
+    <t>M20-9990445</t>
+  </si>
+  <si>
+    <t>2.54mm Pin Header 2x4 THT</t>
+  </si>
+  <si>
+    <t>THT</t>
+  </si>
+  <si>
+    <t>WSOIC-8</t>
+  </si>
+  <si>
+    <t>2.54mm Pin Header 1x4 THT</t>
+  </si>
+  <si>
+    <t>https://uk.rs-online.com/web/p/pcb-headers/6812979/</t>
+  </si>
+  <si>
+    <t>681-2979</t>
+  </si>
+  <si>
+    <t>SC-70-6</t>
+  </si>
+  <si>
+    <t>TPS78233DDCR</t>
+  </si>
+  <si>
+    <t>https://onecall.farnell.com/texas-instruments/tps78233ddcr/ic-ldo-reg-sgl-150ma-5-sot/dp/3007945</t>
+  </si>
+  <si>
+    <t>TSOT-23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32Mbit SPI Flash </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1uF SMD Multilayer Ceramic Capacitor </t>
+  </si>
+  <si>
+    <t>0805</t>
+  </si>
+  <si>
+    <t>0402</t>
+  </si>
+  <si>
+    <t>0603</t>
+  </si>
+  <si>
+    <t>SMA</t>
+  </si>
+  <si>
+    <t>https://uk.rs-online.com/web/p/real-time-clocks/7327582/</t>
+  </si>
+  <si>
+    <t>DS3231SN#</t>
+  </si>
+  <si>
+    <t>732-7582</t>
+  </si>
+  <si>
+    <t>SOIC 16</t>
+  </si>
+  <si>
+    <t>R11, R19, R20</t>
+  </si>
+  <si>
+    <t>R8, R10, R14, R15, R16, R17, R18, R21</t>
+  </si>
+  <si>
+    <t>C2, C6, C7, C9, C10, C11, C12, C13</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Temp. Compensated RTC I2C</t>
   </si>
 </sst>
 </file>
@@ -530,7 +627,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -611,6 +708,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -939,8 +1048,8 @@
   </sheetPr>
   <dimension ref="A1:O172"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:C17"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4498,4 +4607,3764 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId24"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr autoPageBreaks="0"/>
+  </sheetPr>
+  <dimension ref="A1:P173"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.42578125" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="43.7109375" style="11" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="8" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="8" customWidth="1"/>
+    <col min="8" max="8" width="25.85546875" style="11" customWidth="1"/>
+    <col min="9" max="9" width="32.5703125" style="8" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" style="8" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="8"/>
+    <col min="12" max="12" width="15.42578125" style="8" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="8"/>
+    <col min="14" max="14" width="10" style="11" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="35"/>
+      <c r="E2" s="7">
+        <v>1</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="14">
+        <v>1.87</v>
+      </c>
+      <c r="K2" s="7">
+        <v>1</v>
+      </c>
+      <c r="L2" s="15">
+        <f>E2*K29</f>
+        <v>5</v>
+      </c>
+      <c r="M2" s="15">
+        <v>5</v>
+      </c>
+      <c r="N2" s="17">
+        <f t="shared" ref="N2:N21" si="0">M2*J2</f>
+        <v>9.3500000000000014</v>
+      </c>
+      <c r="O2" s="16">
+        <f>N2*1.2</f>
+        <v>11.22</v>
+      </c>
+      <c r="P2"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="35"/>
+      <c r="E3" s="7">
+        <v>2</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="7">
+        <v>2320087</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="14">
+        <v>0.192</v>
+      </c>
+      <c r="K3" s="7">
+        <v>10</v>
+      </c>
+      <c r="L3" s="15">
+        <f>E3*K29</f>
+        <v>10</v>
+      </c>
+      <c r="M3" s="15">
+        <v>10</v>
+      </c>
+      <c r="N3" s="17">
+        <f t="shared" si="0"/>
+        <v>1.92</v>
+      </c>
+      <c r="O3" s="16">
+        <f t="shared" ref="O3:O21" si="1">N3*1.2</f>
+        <v>2.3039999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>128</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="J4" s="14">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="K4" s="7">
+        <v>25</v>
+      </c>
+      <c r="L4" s="15">
+        <f>E4*K29</f>
+        <v>5</v>
+      </c>
+      <c r="M4" s="15">
+        <v>25</v>
+      </c>
+      <c r="N4" s="17">
+        <f>M4*J4</f>
+        <v>9.0250000000000004</v>
+      </c>
+      <c r="O4" s="16">
+        <f>N4*1.2</f>
+        <v>10.83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="35"/>
+      <c r="E5" s="7">
+        <v>1</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="7">
+        <v>2290331</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="14">
+        <v>0.126</v>
+      </c>
+      <c r="K5" s="7">
+        <v>5</v>
+      </c>
+      <c r="L5" s="15">
+        <f>E5*K29</f>
+        <v>5</v>
+      </c>
+      <c r="M5" s="15">
+        <v>5</v>
+      </c>
+      <c r="N5" s="17">
+        <f t="shared" si="0"/>
+        <v>0.63</v>
+      </c>
+      <c r="O5" s="16">
+        <f t="shared" si="1"/>
+        <v>0.75600000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>145</v>
+      </c>
+      <c r="E6" s="7">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="7">
+        <v>3013705</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="14">
+        <v>4.93</v>
+      </c>
+      <c r="K6" s="7">
+        <v>1</v>
+      </c>
+      <c r="L6" s="15">
+        <f>E6*K29</f>
+        <v>5</v>
+      </c>
+      <c r="M6" s="15">
+        <v>5</v>
+      </c>
+      <c r="N6" s="17">
+        <f t="shared" si="0"/>
+        <v>24.65</v>
+      </c>
+      <c r="O6" s="16">
+        <f t="shared" si="1"/>
+        <v>29.58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="E7" s="7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="7">
+        <v>3007945</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="J7" s="14">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="K7" s="7">
+        <v>1</v>
+      </c>
+      <c r="L7" s="15">
+        <f>E7*K29</f>
+        <v>5</v>
+      </c>
+      <c r="M7" s="15">
+        <v>5</v>
+      </c>
+      <c r="N7" s="17">
+        <f>M7*J7</f>
+        <v>3.16</v>
+      </c>
+      <c r="O7" s="16">
+        <f>N7*1.2</f>
+        <v>3.7919999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>141</v>
+      </c>
+      <c r="E8" s="7">
+        <v>1</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="J8" s="14">
+        <v>7.65</v>
+      </c>
+      <c r="K8" s="7">
+        <v>1</v>
+      </c>
+      <c r="L8" s="15">
+        <f>E8*K29</f>
+        <v>5</v>
+      </c>
+      <c r="M8" s="15">
+        <v>5</v>
+      </c>
+      <c r="N8" s="17">
+        <f>M8*J8</f>
+        <v>38.25</v>
+      </c>
+      <c r="O8" s="16">
+        <f>N8*1.2</f>
+        <v>45.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="E9" s="7">
+        <v>1</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="7">
+        <v>2909992</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="J9" s="14">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="K9" s="15">
+        <v>1</v>
+      </c>
+      <c r="L9" s="15">
+        <f>E9*K29</f>
+        <v>5</v>
+      </c>
+      <c r="M9" s="15">
+        <v>5</v>
+      </c>
+      <c r="N9" s="17">
+        <f>M9*J9</f>
+        <v>10.9</v>
+      </c>
+      <c r="O9" s="16">
+        <f>N9*1.2</f>
+        <v>13.08</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="E10" s="7">
+        <v>2</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="7">
+        <v>1658203</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="J10" s="14">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="K10" s="7">
+        <v>5</v>
+      </c>
+      <c r="L10" s="15">
+        <f>E10*K29</f>
+        <v>10</v>
+      </c>
+      <c r="M10" s="15">
+        <v>10</v>
+      </c>
+      <c r="N10" s="17">
+        <f t="shared" si="0"/>
+        <v>5.8</v>
+      </c>
+      <c r="O10" s="16">
+        <f t="shared" si="1"/>
+        <v>6.96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="E11" s="7">
+        <v>8</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="7">
+        <v>2332715</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11" s="14">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="K11" s="7">
+        <v>5</v>
+      </c>
+      <c r="L11" s="15">
+        <f>E11*K29</f>
+        <v>40</v>
+      </c>
+      <c r="M11" s="15">
+        <v>40</v>
+      </c>
+      <c r="N11" s="17">
+        <f t="shared" si="0"/>
+        <v>9.3600000000000012</v>
+      </c>
+      <c r="O11" s="16">
+        <f t="shared" si="1"/>
+        <v>11.232000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="E12" s="7">
+        <v>3</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="7">
+        <v>2346940</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="J12" s="14">
+        <v>0.185</v>
+      </c>
+      <c r="K12" s="7">
+        <v>5</v>
+      </c>
+      <c r="L12" s="15">
+        <f>E12*K29</f>
+        <v>15</v>
+      </c>
+      <c r="M12" s="15">
+        <v>15</v>
+      </c>
+      <c r="N12" s="17">
+        <f>M12*J12</f>
+        <v>2.7749999999999999</v>
+      </c>
+      <c r="O12" s="16">
+        <f>N12*1.2</f>
+        <v>3.3299999999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="E13" s="7">
+        <v>8</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" s="7">
+        <v>1577632</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="J13" s="14">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="K13" s="7">
+        <v>10</v>
+      </c>
+      <c r="L13" s="15">
+        <f>E13*K29</f>
+        <v>40</v>
+      </c>
+      <c r="M13" s="15">
+        <v>40</v>
+      </c>
+      <c r="N13" s="17">
+        <f t="shared" si="0"/>
+        <v>11.240000000000002</v>
+      </c>
+      <c r="O13" s="16">
+        <f t="shared" si="1"/>
+        <v>13.488000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="E14" s="7">
+        <v>6</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="7">
+        <v>9238360</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="J14" s="14">
+        <v>0.02</v>
+      </c>
+      <c r="K14" s="7">
+        <v>10</v>
+      </c>
+      <c r="L14" s="15">
+        <f>E14*K29</f>
+        <v>30</v>
+      </c>
+      <c r="M14" s="15">
+        <v>30</v>
+      </c>
+      <c r="N14" s="17">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="O14" s="16">
+        <f t="shared" si="1"/>
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="E15" s="7">
+        <v>2</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" s="7">
+        <v>9238310</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="J15" s="14">
+        <v>2.06E-2</v>
+      </c>
+      <c r="K15" s="7">
+        <v>10</v>
+      </c>
+      <c r="L15" s="15">
+        <f>E15*K29</f>
+        <v>10</v>
+      </c>
+      <c r="M15" s="15">
+        <v>10</v>
+      </c>
+      <c r="N15" s="17">
+        <f t="shared" si="0"/>
+        <v>0.20600000000000002</v>
+      </c>
+      <c r="O15" s="16">
+        <f t="shared" si="1"/>
+        <v>0.2472</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="E16" s="7">
+        <v>3</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="7">
+        <v>9238484</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="J16" s="14">
+        <v>0.02</v>
+      </c>
+      <c r="K16" s="7">
+        <v>10</v>
+      </c>
+      <c r="L16" s="15">
+        <f>E16*K29</f>
+        <v>15</v>
+      </c>
+      <c r="M16" s="15">
+        <v>15</v>
+      </c>
+      <c r="N16" s="17">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="O16" s="16">
+        <f t="shared" si="1"/>
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="E17" s="7">
+        <v>2</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" s="7">
+        <v>9238530</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="J17" s="14">
+        <v>0.02</v>
+      </c>
+      <c r="K17" s="7">
+        <v>10</v>
+      </c>
+      <c r="L17" s="15">
+        <f>E17*K29</f>
+        <v>10</v>
+      </c>
+      <c r="M17" s="15">
+        <v>10</v>
+      </c>
+      <c r="N17" s="17">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="O17" s="16">
+        <f t="shared" si="1"/>
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="E18" s="7">
+        <v>1</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="7">
+        <v>1669587</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J18" s="14">
+        <v>4.7100000000000003E-2</v>
+      </c>
+      <c r="K18" s="7">
+        <v>10</v>
+      </c>
+      <c r="L18" s="15">
+        <f>E18*K29</f>
+        <v>5</v>
+      </c>
+      <c r="M18" s="15">
+        <v>10</v>
+      </c>
+      <c r="N18" s="17">
+        <f>M18*J18</f>
+        <v>0.47100000000000003</v>
+      </c>
+      <c r="O18" s="16">
+        <f>N18*1.2</f>
+        <v>0.56520000000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="E19" s="7">
+        <v>1</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="7">
+        <v>1169631</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="J19" s="14">
+        <v>3.53</v>
+      </c>
+      <c r="K19" s="7">
+        <v>1</v>
+      </c>
+      <c r="L19" s="15">
+        <f>E19*K29</f>
+        <v>5</v>
+      </c>
+      <c r="M19" s="15">
+        <v>5</v>
+      </c>
+      <c r="N19" s="17">
+        <f>M19*J19</f>
+        <v>17.649999999999999</v>
+      </c>
+      <c r="O19" s="16">
+        <f>N19*1.2</f>
+        <v>21.179999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D20" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="E20" s="7">
+        <v>1</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="7">
+        <v>1022232</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="J20" s="14">
+        <v>0.26</v>
+      </c>
+      <c r="K20" s="7">
+        <v>10</v>
+      </c>
+      <c r="L20" s="15">
+        <f>E20*K29</f>
+        <v>5</v>
+      </c>
+      <c r="M20" s="15">
+        <v>10</v>
+      </c>
+      <c r="N20" s="17">
+        <f t="shared" si="0"/>
+        <v>2.6</v>
+      </c>
+      <c r="O20" s="16">
+        <f t="shared" si="1"/>
+        <v>3.12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B21" s="7"/>
+      <c r="C21" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="E21" s="7">
+        <v>4</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="J21" s="14">
+        <v>0.19</v>
+      </c>
+      <c r="K21" s="7">
+        <v>10</v>
+      </c>
+      <c r="L21" s="15">
+        <f>E21*K29</f>
+        <v>20</v>
+      </c>
+      <c r="M21" s="15">
+        <v>20</v>
+      </c>
+      <c r="N21" s="17">
+        <f t="shared" si="0"/>
+        <v>3.8</v>
+      </c>
+      <c r="O21" s="16">
+        <f t="shared" si="1"/>
+        <v>4.5599999999999996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22" s="7"/>
+      <c r="C22" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="E22" s="7">
+        <v>1</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="J22" s="14">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="K22" s="15">
+        <v>2</v>
+      </c>
+      <c r="L22" s="15">
+        <f>E22*K29</f>
+        <v>5</v>
+      </c>
+      <c r="M22" s="15">
+        <v>6</v>
+      </c>
+      <c r="N22" s="18">
+        <f>M22*J22</f>
+        <v>14.940000000000001</v>
+      </c>
+      <c r="O22" s="16">
+        <f>N22*1.2</f>
+        <v>17.928000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="7">
+        <v>1</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="I23" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="J23" s="14">
+        <v>3.56</v>
+      </c>
+      <c r="K23" s="7">
+        <v>1</v>
+      </c>
+      <c r="L23" s="15">
+        <f>K29*E23</f>
+        <v>5</v>
+      </c>
+      <c r="M23" s="15">
+        <v>0</v>
+      </c>
+      <c r="N23" s="17">
+        <f>M23*J23</f>
+        <v>0</v>
+      </c>
+      <c r="O23" s="16">
+        <f>N23*1.2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="7"/>
+      <c r="C24" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="7">
+        <v>1</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="I24" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="J24" s="14">
+        <v>5.67</v>
+      </c>
+      <c r="K24" s="7">
+        <v>1</v>
+      </c>
+      <c r="L24" s="15">
+        <f>E24*K29</f>
+        <v>5</v>
+      </c>
+      <c r="M24" s="15">
+        <v>0</v>
+      </c>
+      <c r="N24" s="17">
+        <f>M24*J24</f>
+        <v>0</v>
+      </c>
+      <c r="O24" s="16">
+        <f>N24*1.2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="37"/>
+      <c r="M25" s="37"/>
+      <c r="N25" s="38"/>
+      <c r="O25" s="23"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="19"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="21"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="21"/>
+      <c r="N26" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="O26" s="23">
+        <f>SUM(O2:O24)</f>
+        <v>201.39240000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="19"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
+      <c r="L27" s="21"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="22"/>
+      <c r="O27" s="21"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="19"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="21"/>
+      <c r="M28" s="24"/>
+      <c r="N28" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="O28" s="25">
+        <f>O26/K29</f>
+        <v>40.278480000000009</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="19"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="20">
+        <f>SUM(E2:E24)</f>
+        <v>53</v>
+      </c>
+      <c r="F29" s="20"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="K29" s="21">
+        <v>5</v>
+      </c>
+      <c r="L29" s="21"/>
+      <c r="M29" s="21"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="25"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="19"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="20">
+        <f>E29-E24-E23</f>
+        <v>51</v>
+      </c>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="21"/>
+      <c r="O30" s="25"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="19"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="21"/>
+      <c r="M31" s="21"/>
+      <c r="N31" s="21"/>
+      <c r="O31" s="21"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="19"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="21"/>
+      <c r="M32" s="21"/>
+      <c r="N32" s="21"/>
+      <c r="O32" s="25"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="19"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="27"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="21"/>
+      <c r="L33" s="21"/>
+      <c r="M33" s="21"/>
+      <c r="N33" s="21"/>
+      <c r="O33" s="21"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="19"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="21"/>
+      <c r="M34" s="21"/>
+      <c r="N34" s="21"/>
+      <c r="O34" s="21"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="19"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="21"/>
+      <c r="K35" s="21"/>
+      <c r="L35" s="21"/>
+      <c r="M35" s="21"/>
+      <c r="N35" s="21"/>
+      <c r="O35" s="21"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="19"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="21"/>
+      <c r="K36" s="21"/>
+      <c r="L36" s="21"/>
+      <c r="M36" s="21"/>
+      <c r="N36" s="21"/>
+      <c r="O36" s="21"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="19"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="21"/>
+      <c r="K37" s="21"/>
+      <c r="L37" s="21"/>
+      <c r="M37" s="21"/>
+      <c r="N37" s="21"/>
+      <c r="O37" s="21"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="19"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="21"/>
+      <c r="K38" s="21"/>
+      <c r="L38" s="21"/>
+      <c r="M38" s="21"/>
+      <c r="N38" s="21"/>
+      <c r="O38" s="21"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="19"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="27"/>
+      <c r="J39" s="21"/>
+      <c r="K39" s="21"/>
+      <c r="L39" s="21"/>
+      <c r="M39" s="21"/>
+      <c r="N39" s="21"/>
+      <c r="O39" s="21"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" s="19"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="28"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="21"/>
+      <c r="K40" s="21"/>
+      <c r="L40" s="21"/>
+      <c r="M40" s="21"/>
+      <c r="N40" s="21"/>
+      <c r="O40" s="21"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" s="19"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="28"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="21"/>
+      <c r="L41" s="21"/>
+      <c r="M41" s="21"/>
+      <c r="N41" s="21"/>
+      <c r="O41" s="21"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="19"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="28"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="26"/>
+      <c r="J42" s="21"/>
+      <c r="K42" s="21"/>
+      <c r="L42" s="21"/>
+      <c r="M42" s="21"/>
+      <c r="N42" s="21"/>
+      <c r="O42" s="21"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="19"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="28"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="21"/>
+      <c r="K43" s="21"/>
+      <c r="L43" s="21"/>
+      <c r="M43" s="21"/>
+      <c r="N43" s="21"/>
+      <c r="O43" s="21"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="19"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="28"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="21"/>
+      <c r="K44" s="21"/>
+      <c r="L44" s="21"/>
+      <c r="M44" s="21"/>
+      <c r="N44" s="21"/>
+      <c r="O44" s="21"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" s="19"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="28"/>
+      <c r="H45" s="28"/>
+      <c r="I45" s="26"/>
+      <c r="J45" s="21"/>
+      <c r="K45" s="21"/>
+      <c r="L45" s="21"/>
+      <c r="M45" s="21"/>
+      <c r="N45" s="21"/>
+      <c r="O45" s="21"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" s="19"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="28"/>
+      <c r="H46" s="20"/>
+      <c r="I46" s="27"/>
+      <c r="J46" s="21"/>
+      <c r="K46" s="21"/>
+      <c r="L46" s="21"/>
+      <c r="M46" s="21"/>
+      <c r="N46" s="21"/>
+      <c r="O46" s="21"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" s="19"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="28"/>
+      <c r="H47" s="20"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="21"/>
+      <c r="K47" s="21"/>
+      <c r="L47" s="21"/>
+      <c r="M47" s="21"/>
+      <c r="N47" s="21"/>
+      <c r="O47" s="21"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" s="29"/>
+      <c r="B48" s="30"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="29"/>
+      <c r="E48" s="30"/>
+      <c r="F48" s="30"/>
+      <c r="G48" s="30"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="26"/>
+      <c r="J48" s="21"/>
+      <c r="K48" s="21"/>
+      <c r="L48" s="21"/>
+      <c r="M48" s="21"/>
+      <c r="N48" s="21"/>
+      <c r="O48" s="21"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A49" s="19"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="30"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="20"/>
+      <c r="I49" s="26"/>
+      <c r="J49" s="21"/>
+      <c r="K49" s="21"/>
+      <c r="L49" s="21"/>
+      <c r="M49" s="21"/>
+      <c r="N49" s="21"/>
+      <c r="O49" s="21"/>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A50" s="19"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="31"/>
+      <c r="I50" s="26"/>
+      <c r="J50" s="21"/>
+      <c r="K50" s="21"/>
+      <c r="L50" s="21"/>
+      <c r="M50" s="21"/>
+      <c r="N50" s="21"/>
+      <c r="O50" s="21"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A51" s="19"/>
+      <c r="B51" s="20"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="20"/>
+      <c r="H51" s="31"/>
+      <c r="I51" s="26"/>
+      <c r="J51" s="21"/>
+      <c r="K51" s="21"/>
+      <c r="L51" s="21"/>
+      <c r="M51" s="21"/>
+      <c r="N51" s="21"/>
+      <c r="O51" s="21"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52" s="19"/>
+      <c r="B52" s="20"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="20"/>
+      <c r="H52" s="20"/>
+      <c r="I52" s="26"/>
+      <c r="J52" s="21"/>
+      <c r="K52" s="21"/>
+      <c r="L52" s="21"/>
+      <c r="M52" s="21"/>
+      <c r="N52" s="21"/>
+      <c r="O52" s="21"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A53" s="19"/>
+      <c r="B53" s="20"/>
+      <c r="C53" s="19"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="20"/>
+      <c r="G53" s="20"/>
+      <c r="H53" s="20"/>
+      <c r="I53" s="32"/>
+      <c r="J53" s="21"/>
+      <c r="K53" s="21"/>
+      <c r="L53" s="21"/>
+      <c r="M53" s="21"/>
+      <c r="N53" s="21"/>
+      <c r="O53" s="21"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A54" s="19"/>
+      <c r="B54" s="20"/>
+      <c r="C54" s="19"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="20"/>
+      <c r="F54" s="19"/>
+      <c r="G54" s="19"/>
+      <c r="H54" s="19"/>
+      <c r="I54" s="24"/>
+      <c r="J54" s="21"/>
+      <c r="K54" s="21"/>
+      <c r="L54" s="21"/>
+      <c r="M54" s="21"/>
+      <c r="N54" s="21"/>
+      <c r="O54" s="21"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A55" s="19"/>
+      <c r="B55" s="20"/>
+      <c r="C55" s="19"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="20"/>
+      <c r="F55" s="19"/>
+      <c r="G55" s="19"/>
+      <c r="H55" s="19"/>
+      <c r="I55" s="24"/>
+      <c r="J55" s="21"/>
+      <c r="K55" s="21"/>
+      <c r="L55" s="21"/>
+      <c r="M55" s="21"/>
+      <c r="N55" s="21"/>
+      <c r="O55" s="21"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A56" s="19"/>
+      <c r="B56" s="20"/>
+      <c r="C56" s="19"/>
+      <c r="D56" s="19"/>
+      <c r="E56" s="20"/>
+      <c r="F56" s="19"/>
+      <c r="G56" s="19"/>
+      <c r="H56" s="19"/>
+      <c r="I56" s="24"/>
+      <c r="J56" s="21"/>
+      <c r="K56" s="21"/>
+      <c r="L56" s="21"/>
+      <c r="M56" s="21"/>
+      <c r="N56" s="21"/>
+      <c r="O56" s="21"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A57" s="19"/>
+      <c r="B57" s="20"/>
+      <c r="C57" s="19"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="20"/>
+      <c r="F57" s="19"/>
+      <c r="G57" s="19"/>
+      <c r="H57" s="19"/>
+      <c r="I57" s="24"/>
+      <c r="J57" s="21"/>
+      <c r="K57" s="21"/>
+      <c r="L57" s="21"/>
+      <c r="M57" s="21"/>
+      <c r="N57" s="21"/>
+      <c r="O57" s="21"/>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A58" s="21"/>
+      <c r="B58" s="21"/>
+      <c r="C58" s="21"/>
+      <c r="D58" s="21"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="21"/>
+      <c r="G58" s="21"/>
+      <c r="H58" s="21"/>
+      <c r="I58" s="21"/>
+      <c r="J58" s="21"/>
+      <c r="K58" s="21"/>
+      <c r="L58" s="21"/>
+      <c r="M58" s="21"/>
+      <c r="N58" s="21"/>
+      <c r="O58" s="21"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A59" s="21"/>
+      <c r="B59" s="19"/>
+      <c r="C59" s="19"/>
+      <c r="D59" s="19"/>
+      <c r="E59" s="19"/>
+      <c r="F59" s="19"/>
+      <c r="G59" s="19"/>
+      <c r="H59" s="19"/>
+      <c r="I59" s="19"/>
+      <c r="J59" s="21"/>
+      <c r="K59" s="21"/>
+      <c r="L59" s="21"/>
+      <c r="M59" s="21"/>
+      <c r="N59" s="21"/>
+      <c r="O59" s="21"/>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A60" s="19"/>
+      <c r="B60" s="20"/>
+      <c r="C60" s="19"/>
+      <c r="D60" s="19"/>
+      <c r="E60" s="20"/>
+      <c r="F60" s="20"/>
+      <c r="G60" s="20"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="32"/>
+      <c r="J60" s="21"/>
+      <c r="K60" s="21"/>
+      <c r="L60" s="21"/>
+      <c r="M60" s="21"/>
+      <c r="N60" s="21"/>
+      <c r="O60" s="21"/>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A61" s="21"/>
+      <c r="B61" s="21"/>
+      <c r="C61" s="21"/>
+      <c r="D61" s="21"/>
+      <c r="E61" s="21"/>
+      <c r="F61" s="21"/>
+      <c r="G61" s="21"/>
+      <c r="H61" s="21"/>
+      <c r="I61" s="21"/>
+      <c r="J61" s="21"/>
+      <c r="K61" s="21"/>
+      <c r="L61" s="21"/>
+      <c r="M61" s="21"/>
+      <c r="N61" s="21"/>
+      <c r="O61" s="21"/>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A62" s="21"/>
+      <c r="B62" s="21"/>
+      <c r="C62" s="21"/>
+      <c r="D62" s="21"/>
+      <c r="E62" s="21"/>
+      <c r="F62" s="21"/>
+      <c r="G62" s="21"/>
+      <c r="H62" s="21"/>
+      <c r="I62" s="21"/>
+      <c r="J62" s="21"/>
+      <c r="K62" s="21"/>
+      <c r="L62" s="21"/>
+      <c r="M62" s="21"/>
+      <c r="N62" s="21"/>
+      <c r="O62" s="21"/>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A63" s="21"/>
+      <c r="B63" s="21"/>
+      <c r="C63" s="21"/>
+      <c r="D63" s="21"/>
+      <c r="E63" s="21"/>
+      <c r="F63" s="21"/>
+      <c r="G63" s="21"/>
+      <c r="H63" s="21"/>
+      <c r="I63" s="21"/>
+      <c r="J63" s="21"/>
+      <c r="K63" s="21"/>
+      <c r="L63" s="21"/>
+      <c r="M63" s="21"/>
+      <c r="N63" s="21"/>
+      <c r="O63" s="21"/>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A64" s="21"/>
+      <c r="B64" s="21"/>
+      <c r="C64" s="21"/>
+      <c r="D64" s="21"/>
+      <c r="E64" s="21"/>
+      <c r="F64" s="21"/>
+      <c r="G64" s="21"/>
+      <c r="H64" s="21"/>
+      <c r="I64" s="21"/>
+      <c r="J64" s="21"/>
+      <c r="K64" s="21"/>
+      <c r="L64" s="21"/>
+      <c r="M64" s="21"/>
+      <c r="N64" s="21"/>
+      <c r="O64" s="21"/>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A65" s="21"/>
+      <c r="B65" s="21"/>
+      <c r="C65" s="21"/>
+      <c r="D65" s="21"/>
+      <c r="E65" s="21"/>
+      <c r="F65" s="21"/>
+      <c r="G65" s="21"/>
+      <c r="H65" s="21"/>
+      <c r="I65" s="21"/>
+      <c r="J65" s="21"/>
+      <c r="K65" s="21"/>
+      <c r="L65" s="21"/>
+      <c r="M65" s="21"/>
+      <c r="N65" s="21"/>
+      <c r="O65" s="21"/>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A66" s="21"/>
+      <c r="B66" s="21"/>
+      <c r="C66" s="21"/>
+      <c r="D66" s="21"/>
+      <c r="E66" s="21"/>
+      <c r="F66" s="21"/>
+      <c r="G66" s="21"/>
+      <c r="H66" s="21"/>
+      <c r="I66" s="21"/>
+      <c r="J66" s="21"/>
+      <c r="K66" s="21"/>
+      <c r="L66" s="21"/>
+      <c r="M66" s="21"/>
+      <c r="N66" s="21"/>
+      <c r="O66" s="21"/>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A67" s="21"/>
+      <c r="B67" s="21"/>
+      <c r="C67" s="21"/>
+      <c r="D67" s="21"/>
+      <c r="E67" s="21"/>
+      <c r="F67" s="21"/>
+      <c r="G67" s="21"/>
+      <c r="H67" s="21"/>
+      <c r="I67" s="21"/>
+      <c r="J67" s="21"/>
+      <c r="K67" s="21"/>
+      <c r="L67" s="21"/>
+      <c r="M67" s="21"/>
+      <c r="N67" s="21"/>
+      <c r="O67" s="21"/>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A68" s="21"/>
+      <c r="B68" s="21"/>
+      <c r="C68" s="21"/>
+      <c r="D68" s="21"/>
+      <c r="E68" s="21"/>
+      <c r="F68" s="21"/>
+      <c r="G68" s="21"/>
+      <c r="H68" s="21"/>
+      <c r="I68" s="21"/>
+      <c r="J68" s="21"/>
+      <c r="K68" s="21"/>
+      <c r="L68" s="21"/>
+      <c r="M68" s="21"/>
+      <c r="N68" s="21"/>
+      <c r="O68" s="21"/>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A69" s="21"/>
+      <c r="B69" s="21"/>
+      <c r="C69" s="21"/>
+      <c r="D69" s="21"/>
+      <c r="E69" s="21"/>
+      <c r="F69" s="21"/>
+      <c r="G69" s="21"/>
+      <c r="H69" s="21"/>
+      <c r="I69" s="21"/>
+      <c r="J69" s="21"/>
+      <c r="K69" s="21"/>
+      <c r="L69" s="21"/>
+      <c r="M69" s="21"/>
+      <c r="N69" s="21"/>
+      <c r="O69" s="21"/>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A70" s="21"/>
+      <c r="B70" s="21"/>
+      <c r="C70" s="21"/>
+      <c r="D70" s="21"/>
+      <c r="E70" s="21"/>
+      <c r="F70" s="21"/>
+      <c r="G70" s="21"/>
+      <c r="H70" s="21"/>
+      <c r="I70" s="21"/>
+      <c r="J70" s="21"/>
+      <c r="K70" s="21"/>
+      <c r="L70" s="21"/>
+      <c r="M70" s="21"/>
+      <c r="N70" s="21"/>
+      <c r="O70" s="21"/>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A71" s="21"/>
+      <c r="B71" s="21"/>
+      <c r="C71" s="21"/>
+      <c r="D71" s="21"/>
+      <c r="E71" s="21"/>
+      <c r="F71" s="21"/>
+      <c r="G71" s="21"/>
+      <c r="H71" s="21"/>
+      <c r="I71" s="21"/>
+      <c r="J71" s="21"/>
+      <c r="K71" s="21"/>
+      <c r="L71" s="21"/>
+      <c r="M71" s="21"/>
+      <c r="N71" s="21"/>
+      <c r="O71" s="21"/>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A72" s="21"/>
+      <c r="B72" s="21"/>
+      <c r="C72" s="21"/>
+      <c r="D72" s="21"/>
+      <c r="E72" s="21"/>
+      <c r="F72" s="21"/>
+      <c r="G72" s="21"/>
+      <c r="H72" s="21"/>
+      <c r="I72" s="21"/>
+      <c r="J72" s="21"/>
+      <c r="K72" s="21"/>
+      <c r="L72" s="21"/>
+      <c r="M72" s="21"/>
+      <c r="N72" s="21"/>
+      <c r="O72" s="21"/>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A73" s="21"/>
+      <c r="B73" s="21"/>
+      <c r="C73" s="21"/>
+      <c r="D73" s="21"/>
+      <c r="E73" s="21"/>
+      <c r="F73" s="21"/>
+      <c r="G73" s="21"/>
+      <c r="H73" s="21"/>
+      <c r="I73" s="21"/>
+      <c r="J73" s="21"/>
+      <c r="K73" s="21"/>
+      <c r="L73" s="21"/>
+      <c r="M73" s="21"/>
+      <c r="N73" s="21"/>
+      <c r="O73" s="21"/>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A74" s="21"/>
+      <c r="B74" s="21"/>
+      <c r="C74" s="21"/>
+      <c r="D74" s="21"/>
+      <c r="E74" s="21"/>
+      <c r="F74" s="21"/>
+      <c r="G74" s="21"/>
+      <c r="H74" s="21"/>
+      <c r="I74" s="21"/>
+      <c r="J74" s="21"/>
+      <c r="K74" s="21"/>
+      <c r="L74" s="21"/>
+      <c r="M74" s="21"/>
+      <c r="N74" s="21"/>
+      <c r="O74" s="21"/>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A75" s="21"/>
+      <c r="B75" s="21"/>
+      <c r="C75" s="21"/>
+      <c r="D75" s="21"/>
+      <c r="E75" s="21"/>
+      <c r="F75" s="21"/>
+      <c r="G75" s="21"/>
+      <c r="H75" s="21"/>
+      <c r="I75" s="21"/>
+      <c r="J75" s="21"/>
+      <c r="K75" s="21"/>
+      <c r="L75" s="21"/>
+      <c r="M75" s="21"/>
+      <c r="N75" s="21"/>
+      <c r="O75" s="21"/>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A76" s="21"/>
+      <c r="B76" s="21"/>
+      <c r="C76" s="21"/>
+      <c r="D76" s="21"/>
+      <c r="E76" s="21"/>
+      <c r="F76" s="21"/>
+      <c r="G76" s="21"/>
+      <c r="H76" s="21"/>
+      <c r="I76" s="21"/>
+      <c r="J76" s="21"/>
+      <c r="K76" s="21"/>
+      <c r="L76" s="21"/>
+      <c r="M76" s="21"/>
+      <c r="N76" s="21"/>
+      <c r="O76" s="21"/>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A77" s="21"/>
+      <c r="B77" s="21"/>
+      <c r="C77" s="21"/>
+      <c r="D77" s="21"/>
+      <c r="E77" s="21"/>
+      <c r="F77" s="21"/>
+      <c r="G77" s="21"/>
+      <c r="H77" s="21"/>
+      <c r="I77" s="21"/>
+      <c r="J77" s="21"/>
+      <c r="K77" s="21"/>
+      <c r="L77" s="21"/>
+      <c r="M77" s="21"/>
+      <c r="N77" s="21"/>
+      <c r="O77" s="21"/>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A78" s="21"/>
+      <c r="B78" s="21"/>
+      <c r="C78" s="21"/>
+      <c r="D78" s="21"/>
+      <c r="E78" s="21"/>
+      <c r="F78" s="21"/>
+      <c r="G78" s="21"/>
+      <c r="H78" s="21"/>
+      <c r="I78" s="21"/>
+      <c r="J78" s="21"/>
+      <c r="K78" s="21"/>
+      <c r="L78" s="21"/>
+      <c r="M78" s="21"/>
+      <c r="N78" s="21"/>
+      <c r="O78" s="21"/>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A79" s="21"/>
+      <c r="B79" s="21"/>
+      <c r="C79" s="21"/>
+      <c r="D79" s="21"/>
+      <c r="E79" s="21"/>
+      <c r="F79" s="21"/>
+      <c r="G79" s="21"/>
+      <c r="H79" s="21"/>
+      <c r="I79" s="21"/>
+      <c r="J79" s="21"/>
+      <c r="K79" s="21"/>
+      <c r="L79" s="21"/>
+      <c r="M79" s="21"/>
+      <c r="N79" s="21"/>
+      <c r="O79" s="21"/>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A80" s="21"/>
+      <c r="B80" s="21"/>
+      <c r="C80" s="21"/>
+      <c r="D80" s="21"/>
+      <c r="E80" s="21"/>
+      <c r="F80" s="21"/>
+      <c r="G80" s="21"/>
+      <c r="H80" s="21"/>
+      <c r="I80" s="21"/>
+      <c r="J80" s="21"/>
+      <c r="K80" s="21"/>
+      <c r="L80" s="21"/>
+      <c r="M80" s="21"/>
+      <c r="N80" s="21"/>
+      <c r="O80" s="21"/>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A81" s="21"/>
+      <c r="B81" s="21"/>
+      <c r="C81" s="21"/>
+      <c r="D81" s="21"/>
+      <c r="E81" s="21"/>
+      <c r="F81" s="21"/>
+      <c r="G81" s="21"/>
+      <c r="H81" s="21"/>
+      <c r="I81" s="21"/>
+      <c r="J81" s="21"/>
+      <c r="K81" s="21"/>
+      <c r="L81" s="21"/>
+      <c r="M81" s="21"/>
+      <c r="N81" s="21"/>
+      <c r="O81" s="21"/>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A82" s="21"/>
+      <c r="B82" s="21"/>
+      <c r="C82" s="21"/>
+      <c r="D82" s="21"/>
+      <c r="E82" s="21"/>
+      <c r="F82" s="21"/>
+      <c r="G82" s="21"/>
+      <c r="H82" s="21"/>
+      <c r="I82" s="21"/>
+      <c r="J82" s="21"/>
+      <c r="K82" s="21"/>
+      <c r="L82" s="21"/>
+      <c r="M82" s="21"/>
+      <c r="N82" s="21"/>
+      <c r="O82" s="21"/>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A83" s="21"/>
+      <c r="B83" s="21"/>
+      <c r="C83" s="21"/>
+      <c r="D83" s="21"/>
+      <c r="E83" s="21"/>
+      <c r="F83" s="21"/>
+      <c r="G83" s="21"/>
+      <c r="H83" s="21"/>
+      <c r="I83" s="21"/>
+      <c r="J83" s="21"/>
+      <c r="K83" s="21"/>
+      <c r="L83" s="21"/>
+      <c r="M83" s="21"/>
+      <c r="N83" s="21"/>
+      <c r="O83" s="21"/>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A84" s="21"/>
+      <c r="B84" s="21"/>
+      <c r="C84" s="21"/>
+      <c r="D84" s="21"/>
+      <c r="E84" s="21"/>
+      <c r="F84" s="21"/>
+      <c r="G84" s="21"/>
+      <c r="H84" s="21"/>
+      <c r="I84" s="21"/>
+      <c r="J84" s="21"/>
+      <c r="K84" s="21"/>
+      <c r="L84" s="21"/>
+      <c r="M84" s="21"/>
+      <c r="N84" s="21"/>
+      <c r="O84" s="21"/>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A85" s="21"/>
+      <c r="B85" s="21"/>
+      <c r="C85" s="21"/>
+      <c r="D85" s="21"/>
+      <c r="E85" s="21"/>
+      <c r="F85" s="21"/>
+      <c r="G85" s="21"/>
+      <c r="H85" s="21"/>
+      <c r="I85" s="21"/>
+      <c r="J85" s="21"/>
+      <c r="K85" s="21"/>
+      <c r="L85" s="21"/>
+      <c r="M85" s="21"/>
+      <c r="N85" s="21"/>
+      <c r="O85" s="21"/>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A86" s="21"/>
+      <c r="B86" s="21"/>
+      <c r="C86" s="21"/>
+      <c r="D86" s="21"/>
+      <c r="E86" s="21"/>
+      <c r="F86" s="21"/>
+      <c r="G86" s="21"/>
+      <c r="H86" s="21"/>
+      <c r="I86" s="21"/>
+      <c r="J86" s="21"/>
+      <c r="K86" s="21"/>
+      <c r="L86" s="21"/>
+      <c r="M86" s="21"/>
+      <c r="N86" s="21"/>
+      <c r="O86" s="21"/>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A87" s="21"/>
+      <c r="B87" s="21"/>
+      <c r="C87" s="21"/>
+      <c r="D87" s="21"/>
+      <c r="E87" s="21"/>
+      <c r="F87" s="21"/>
+      <c r="G87" s="21"/>
+      <c r="H87" s="21"/>
+      <c r="I87" s="21"/>
+      <c r="J87" s="21"/>
+      <c r="K87" s="21"/>
+      <c r="L87" s="21"/>
+      <c r="M87" s="21"/>
+      <c r="N87" s="21"/>
+      <c r="O87" s="21"/>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A88" s="21"/>
+      <c r="B88" s="21"/>
+      <c r="C88" s="21"/>
+      <c r="D88" s="21"/>
+      <c r="E88" s="21"/>
+      <c r="F88" s="21"/>
+      <c r="G88" s="21"/>
+      <c r="H88" s="21"/>
+      <c r="I88" s="21"/>
+      <c r="J88" s="21"/>
+      <c r="K88" s="21"/>
+      <c r="L88" s="21"/>
+      <c r="M88" s="21"/>
+      <c r="N88" s="21"/>
+      <c r="O88" s="21"/>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A89" s="21"/>
+      <c r="B89" s="21"/>
+      <c r="C89" s="21"/>
+      <c r="D89" s="21"/>
+      <c r="E89" s="21"/>
+      <c r="F89" s="21"/>
+      <c r="G89" s="21"/>
+      <c r="H89" s="21"/>
+      <c r="I89" s="21"/>
+      <c r="J89" s="21"/>
+      <c r="K89" s="21"/>
+      <c r="L89" s="21"/>
+      <c r="M89" s="21"/>
+      <c r="N89" s="21"/>
+      <c r="O89" s="21"/>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A90" s="21"/>
+      <c r="B90" s="21"/>
+      <c r="C90" s="21"/>
+      <c r="D90" s="21"/>
+      <c r="E90" s="21"/>
+      <c r="F90" s="21"/>
+      <c r="G90" s="21"/>
+      <c r="H90" s="21"/>
+      <c r="I90" s="21"/>
+      <c r="J90" s="21"/>
+      <c r="K90" s="21"/>
+      <c r="L90" s="21"/>
+      <c r="M90" s="21"/>
+      <c r="N90" s="21"/>
+      <c r="O90" s="21"/>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A91" s="21"/>
+      <c r="B91" s="21"/>
+      <c r="C91" s="21"/>
+      <c r="D91" s="21"/>
+      <c r="E91" s="21"/>
+      <c r="F91" s="21"/>
+      <c r="G91" s="21"/>
+      <c r="H91" s="21"/>
+      <c r="I91" s="21"/>
+      <c r="J91" s="21"/>
+      <c r="K91" s="21"/>
+      <c r="L91" s="21"/>
+      <c r="M91" s="21"/>
+      <c r="N91" s="21"/>
+      <c r="O91" s="21"/>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A92" s="21"/>
+      <c r="B92" s="21"/>
+      <c r="C92" s="21"/>
+      <c r="D92" s="21"/>
+      <c r="E92" s="21"/>
+      <c r="F92" s="21"/>
+      <c r="G92" s="21"/>
+      <c r="H92" s="21"/>
+      <c r="I92" s="21"/>
+      <c r="J92" s="21"/>
+      <c r="K92" s="21"/>
+      <c r="L92" s="21"/>
+      <c r="M92" s="21"/>
+      <c r="N92" s="21"/>
+      <c r="O92" s="21"/>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A93" s="21"/>
+      <c r="B93" s="21"/>
+      <c r="C93" s="21"/>
+      <c r="D93" s="21"/>
+      <c r="E93" s="21"/>
+      <c r="F93" s="21"/>
+      <c r="G93" s="21"/>
+      <c r="H93" s="21"/>
+      <c r="I93" s="21"/>
+      <c r="J93" s="21"/>
+      <c r="K93" s="21"/>
+      <c r="L93" s="21"/>
+      <c r="M93" s="21"/>
+      <c r="N93" s="21"/>
+      <c r="O93" s="21"/>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A94" s="21"/>
+      <c r="B94" s="21"/>
+      <c r="C94" s="21"/>
+      <c r="D94" s="21"/>
+      <c r="E94" s="21"/>
+      <c r="F94" s="21"/>
+      <c r="G94" s="21"/>
+      <c r="H94" s="21"/>
+      <c r="I94" s="21"/>
+      <c r="J94" s="21"/>
+      <c r="K94" s="21"/>
+      <c r="L94" s="21"/>
+      <c r="M94" s="21"/>
+      <c r="N94" s="21"/>
+      <c r="O94" s="21"/>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A95" s="21"/>
+      <c r="B95" s="21"/>
+      <c r="C95" s="21"/>
+      <c r="D95" s="21"/>
+      <c r="E95" s="21"/>
+      <c r="F95" s="21"/>
+      <c r="G95" s="21"/>
+      <c r="H95" s="21"/>
+      <c r="I95" s="21"/>
+      <c r="J95" s="21"/>
+      <c r="K95" s="21"/>
+      <c r="L95" s="21"/>
+      <c r="M95" s="21"/>
+      <c r="N95" s="21"/>
+      <c r="O95" s="21"/>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A96" s="21"/>
+      <c r="B96" s="21"/>
+      <c r="C96" s="21"/>
+      <c r="D96" s="21"/>
+      <c r="E96" s="21"/>
+      <c r="F96" s="21"/>
+      <c r="G96" s="21"/>
+      <c r="H96" s="21"/>
+      <c r="I96" s="21"/>
+      <c r="J96" s="21"/>
+      <c r="K96" s="21"/>
+      <c r="L96" s="21"/>
+      <c r="M96" s="21"/>
+      <c r="N96" s="21"/>
+      <c r="O96" s="21"/>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A97" s="21"/>
+      <c r="B97" s="21"/>
+      <c r="C97" s="21"/>
+      <c r="D97" s="21"/>
+      <c r="E97" s="21"/>
+      <c r="F97" s="21"/>
+      <c r="G97" s="21"/>
+      <c r="H97" s="21"/>
+      <c r="I97" s="21"/>
+      <c r="J97" s="21"/>
+      <c r="K97" s="21"/>
+      <c r="L97" s="21"/>
+      <c r="M97" s="21"/>
+      <c r="N97" s="21"/>
+      <c r="O97" s="21"/>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A98" s="21"/>
+      <c r="B98" s="21"/>
+      <c r="C98" s="21"/>
+      <c r="D98" s="21"/>
+      <c r="E98" s="21"/>
+      <c r="F98" s="21"/>
+      <c r="G98" s="21"/>
+      <c r="H98" s="21"/>
+      <c r="I98" s="21"/>
+      <c r="J98" s="21"/>
+      <c r="K98" s="21"/>
+      <c r="L98" s="21"/>
+      <c r="M98" s="21"/>
+      <c r="N98" s="21"/>
+      <c r="O98" s="21"/>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A99" s="21"/>
+      <c r="B99" s="21"/>
+      <c r="C99" s="21"/>
+      <c r="D99" s="21"/>
+      <c r="E99" s="21"/>
+      <c r="F99" s="21"/>
+      <c r="G99" s="21"/>
+      <c r="H99" s="21"/>
+      <c r="I99" s="21"/>
+      <c r="J99" s="21"/>
+      <c r="K99" s="21"/>
+      <c r="L99" s="21"/>
+      <c r="M99" s="21"/>
+      <c r="N99" s="21"/>
+      <c r="O99" s="21"/>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A100" s="21"/>
+      <c r="B100" s="21"/>
+      <c r="C100" s="21"/>
+      <c r="D100" s="21"/>
+      <c r="E100" s="21"/>
+      <c r="F100" s="21"/>
+      <c r="G100" s="21"/>
+      <c r="H100" s="21"/>
+      <c r="I100" s="21"/>
+      <c r="J100" s="21"/>
+      <c r="K100" s="21"/>
+      <c r="L100" s="21"/>
+      <c r="M100" s="21"/>
+      <c r="N100" s="21"/>
+      <c r="O100" s="21"/>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A101" s="21"/>
+      <c r="B101" s="21"/>
+      <c r="C101" s="21"/>
+      <c r="D101" s="21"/>
+      <c r="E101" s="21"/>
+      <c r="F101" s="21"/>
+      <c r="G101" s="21"/>
+      <c r="H101" s="21"/>
+      <c r="I101" s="21"/>
+      <c r="J101" s="21"/>
+      <c r="K101" s="21"/>
+      <c r="L101" s="21"/>
+      <c r="M101" s="21"/>
+      <c r="N101" s="21"/>
+      <c r="O101" s="21"/>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A102" s="21"/>
+      <c r="B102" s="21"/>
+      <c r="C102" s="21"/>
+      <c r="D102" s="21"/>
+      <c r="E102" s="21"/>
+      <c r="F102" s="21"/>
+      <c r="G102" s="21"/>
+      <c r="H102" s="21"/>
+      <c r="I102" s="21"/>
+      <c r="J102" s="21"/>
+      <c r="K102" s="21"/>
+      <c r="L102" s="21"/>
+      <c r="M102" s="21"/>
+      <c r="N102" s="21"/>
+      <c r="O102" s="21"/>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A103" s="21"/>
+      <c r="B103" s="21"/>
+      <c r="C103" s="21"/>
+      <c r="D103" s="21"/>
+      <c r="E103" s="21"/>
+      <c r="F103" s="21"/>
+      <c r="G103" s="21"/>
+      <c r="H103" s="21"/>
+      <c r="I103" s="21"/>
+      <c r="J103" s="21"/>
+      <c r="K103" s="21"/>
+      <c r="L103" s="21"/>
+      <c r="M103" s="21"/>
+      <c r="N103" s="21"/>
+      <c r="O103" s="21"/>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A104" s="21"/>
+      <c r="B104" s="21"/>
+      <c r="C104" s="21"/>
+      <c r="D104" s="21"/>
+      <c r="E104" s="21"/>
+      <c r="F104" s="21"/>
+      <c r="G104" s="21"/>
+      <c r="H104" s="21"/>
+      <c r="I104" s="21"/>
+      <c r="J104" s="21"/>
+      <c r="K104" s="21"/>
+      <c r="L104" s="21"/>
+      <c r="M104" s="21"/>
+      <c r="N104" s="21"/>
+      <c r="O104" s="21"/>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A105" s="21"/>
+      <c r="B105" s="21"/>
+      <c r="C105" s="21"/>
+      <c r="D105" s="21"/>
+      <c r="E105" s="21"/>
+      <c r="F105" s="21"/>
+      <c r="G105" s="21"/>
+      <c r="H105" s="21"/>
+      <c r="I105" s="21"/>
+      <c r="J105" s="21"/>
+      <c r="K105" s="21"/>
+      <c r="L105" s="21"/>
+      <c r="M105" s="21"/>
+      <c r="N105" s="21"/>
+      <c r="O105" s="21"/>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A106" s="21"/>
+      <c r="B106" s="21"/>
+      <c r="C106" s="21"/>
+      <c r="D106" s="21"/>
+      <c r="E106" s="21"/>
+      <c r="F106" s="21"/>
+      <c r="G106" s="21"/>
+      <c r="H106" s="21"/>
+      <c r="I106" s="21"/>
+      <c r="J106" s="21"/>
+      <c r="K106" s="21"/>
+      <c r="L106" s="21"/>
+      <c r="M106" s="21"/>
+      <c r="N106" s="21"/>
+      <c r="O106" s="21"/>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A107" s="21"/>
+      <c r="B107" s="21"/>
+      <c r="C107" s="21"/>
+      <c r="D107" s="21"/>
+      <c r="E107" s="21"/>
+      <c r="F107" s="21"/>
+      <c r="G107" s="21"/>
+      <c r="H107" s="21"/>
+      <c r="I107" s="21"/>
+      <c r="J107" s="21"/>
+      <c r="K107" s="21"/>
+      <c r="L107" s="21"/>
+      <c r="M107" s="21"/>
+      <c r="N107" s="21"/>
+      <c r="O107" s="21"/>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A108" s="21"/>
+      <c r="B108" s="21"/>
+      <c r="C108" s="21"/>
+      <c r="D108" s="21"/>
+      <c r="E108" s="21"/>
+      <c r="F108" s="21"/>
+      <c r="G108" s="21"/>
+      <c r="H108" s="21"/>
+      <c r="I108" s="21"/>
+      <c r="J108" s="21"/>
+      <c r="K108" s="21"/>
+      <c r="L108" s="21"/>
+      <c r="M108" s="21"/>
+      <c r="N108" s="21"/>
+      <c r="O108" s="21"/>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A109" s="21"/>
+      <c r="B109" s="21"/>
+      <c r="C109" s="21"/>
+      <c r="D109" s="21"/>
+      <c r="E109" s="21"/>
+      <c r="F109" s="21"/>
+      <c r="G109" s="21"/>
+      <c r="H109" s="21"/>
+      <c r="I109" s="21"/>
+      <c r="J109" s="21"/>
+      <c r="K109" s="21"/>
+      <c r="L109" s="21"/>
+      <c r="M109" s="21"/>
+      <c r="N109" s="21"/>
+      <c r="O109" s="21"/>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A110" s="21"/>
+      <c r="B110" s="21"/>
+      <c r="C110" s="21"/>
+      <c r="D110" s="21"/>
+      <c r="E110" s="21"/>
+      <c r="F110" s="21"/>
+      <c r="G110" s="21"/>
+      <c r="H110" s="21"/>
+      <c r="I110" s="21"/>
+      <c r="J110" s="21"/>
+      <c r="K110" s="21"/>
+      <c r="L110" s="21"/>
+      <c r="M110" s="21"/>
+      <c r="N110" s="21"/>
+      <c r="O110" s="21"/>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A111" s="21"/>
+      <c r="B111" s="21"/>
+      <c r="C111" s="21"/>
+      <c r="D111" s="21"/>
+      <c r="E111" s="21"/>
+      <c r="F111" s="21"/>
+      <c r="G111" s="21"/>
+      <c r="H111" s="21"/>
+      <c r="I111" s="21"/>
+      <c r="J111" s="21"/>
+      <c r="K111" s="21"/>
+      <c r="L111" s="21"/>
+      <c r="M111" s="21"/>
+      <c r="N111" s="21"/>
+      <c r="O111" s="21"/>
+    </row>
+    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A112" s="21"/>
+      <c r="B112" s="21"/>
+      <c r="C112" s="21"/>
+      <c r="D112" s="21"/>
+      <c r="E112" s="21"/>
+      <c r="F112" s="21"/>
+      <c r="G112" s="21"/>
+      <c r="H112" s="21"/>
+      <c r="I112" s="21"/>
+      <c r="J112" s="21"/>
+      <c r="K112" s="21"/>
+      <c r="L112" s="21"/>
+      <c r="M112" s="21"/>
+      <c r="N112" s="21"/>
+      <c r="O112" s="21"/>
+    </row>
+    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A113" s="21"/>
+      <c r="B113" s="21"/>
+      <c r="C113" s="21"/>
+      <c r="D113" s="21"/>
+      <c r="E113" s="21"/>
+      <c r="F113" s="21"/>
+      <c r="G113" s="21"/>
+      <c r="H113" s="21"/>
+      <c r="I113" s="21"/>
+      <c r="J113" s="21"/>
+      <c r="K113" s="21"/>
+      <c r="L113" s="21"/>
+      <c r="M113" s="21"/>
+      <c r="N113" s="21"/>
+      <c r="O113" s="21"/>
+    </row>
+    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A114" s="21"/>
+      <c r="B114" s="21"/>
+      <c r="C114" s="21"/>
+      <c r="D114" s="21"/>
+      <c r="E114" s="21"/>
+      <c r="F114" s="21"/>
+      <c r="G114" s="21"/>
+      <c r="H114" s="21"/>
+      <c r="I114" s="21"/>
+      <c r="J114" s="21"/>
+      <c r="K114" s="21"/>
+      <c r="L114" s="21"/>
+      <c r="M114" s="21"/>
+      <c r="N114" s="21"/>
+      <c r="O114" s="21"/>
+    </row>
+    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A115" s="21"/>
+      <c r="B115" s="21"/>
+      <c r="C115" s="21"/>
+      <c r="D115" s="21"/>
+      <c r="E115" s="21"/>
+      <c r="F115" s="21"/>
+      <c r="G115" s="21"/>
+      <c r="H115" s="21"/>
+      <c r="I115" s="21"/>
+      <c r="J115" s="21"/>
+      <c r="K115" s="21"/>
+      <c r="L115" s="21"/>
+      <c r="M115" s="21"/>
+      <c r="N115" s="21"/>
+      <c r="O115" s="21"/>
+    </row>
+    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A116" s="21"/>
+      <c r="B116" s="21"/>
+      <c r="C116" s="21"/>
+      <c r="D116" s="21"/>
+      <c r="E116" s="21"/>
+      <c r="F116" s="21"/>
+      <c r="G116" s="21"/>
+      <c r="H116" s="21"/>
+      <c r="I116" s="21"/>
+      <c r="J116" s="21"/>
+      <c r="K116" s="21"/>
+      <c r="L116" s="21"/>
+      <c r="M116" s="21"/>
+      <c r="N116" s="21"/>
+      <c r="O116" s="21"/>
+    </row>
+    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A117" s="21"/>
+      <c r="B117" s="21"/>
+      <c r="C117" s="21"/>
+      <c r="D117" s="21"/>
+      <c r="E117" s="21"/>
+      <c r="F117" s="21"/>
+      <c r="G117" s="21"/>
+      <c r="H117" s="21"/>
+      <c r="I117" s="21"/>
+      <c r="J117" s="21"/>
+      <c r="K117" s="21"/>
+      <c r="L117" s="21"/>
+      <c r="M117" s="21"/>
+      <c r="N117" s="21"/>
+      <c r="O117" s="21"/>
+    </row>
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A118" s="21"/>
+      <c r="B118" s="21"/>
+      <c r="C118" s="21"/>
+      <c r="D118" s="21"/>
+      <c r="E118" s="21"/>
+      <c r="F118" s="21"/>
+      <c r="G118" s="21"/>
+      <c r="H118" s="21"/>
+      <c r="I118" s="21"/>
+      <c r="J118" s="21"/>
+      <c r="K118" s="21"/>
+      <c r="L118" s="21"/>
+      <c r="M118" s="21"/>
+      <c r="N118" s="21"/>
+      <c r="O118" s="21"/>
+    </row>
+    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A119" s="21"/>
+      <c r="B119" s="21"/>
+      <c r="C119" s="21"/>
+      <c r="D119" s="21"/>
+      <c r="E119" s="21"/>
+      <c r="F119" s="21"/>
+      <c r="G119" s="21"/>
+      <c r="H119" s="21"/>
+      <c r="I119" s="21"/>
+      <c r="J119" s="21"/>
+      <c r="K119" s="21"/>
+      <c r="L119" s="21"/>
+      <c r="M119" s="21"/>
+      <c r="N119" s="21"/>
+      <c r="O119" s="21"/>
+    </row>
+    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A120" s="21"/>
+      <c r="B120" s="21"/>
+      <c r="C120" s="21"/>
+      <c r="D120" s="21"/>
+      <c r="E120" s="21"/>
+      <c r="F120" s="21"/>
+      <c r="G120" s="21"/>
+      <c r="H120" s="21"/>
+      <c r="I120" s="21"/>
+      <c r="J120" s="21"/>
+      <c r="K120" s="21"/>
+      <c r="L120" s="21"/>
+      <c r="M120" s="21"/>
+      <c r="N120" s="21"/>
+      <c r="O120" s="21"/>
+    </row>
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A121" s="21"/>
+      <c r="B121" s="21"/>
+      <c r="C121" s="21"/>
+      <c r="D121" s="21"/>
+      <c r="E121" s="21"/>
+      <c r="F121" s="21"/>
+      <c r="G121" s="21"/>
+      <c r="H121" s="21"/>
+      <c r="I121" s="21"/>
+      <c r="J121" s="21"/>
+      <c r="K121" s="21"/>
+      <c r="L121" s="21"/>
+      <c r="M121" s="21"/>
+      <c r="N121" s="21"/>
+      <c r="O121" s="21"/>
+    </row>
+    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A122" s="21"/>
+      <c r="B122" s="21"/>
+      <c r="C122" s="21"/>
+      <c r="D122" s="21"/>
+      <c r="E122" s="21"/>
+      <c r="F122" s="21"/>
+      <c r="G122" s="21"/>
+      <c r="H122" s="21"/>
+      <c r="I122" s="21"/>
+      <c r="J122" s="21"/>
+      <c r="K122" s="21"/>
+      <c r="L122" s="21"/>
+      <c r="M122" s="21"/>
+      <c r="N122" s="21"/>
+      <c r="O122" s="21"/>
+    </row>
+    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A123" s="21"/>
+      <c r="B123" s="21"/>
+      <c r="C123" s="21"/>
+      <c r="D123" s="21"/>
+      <c r="E123" s="21"/>
+      <c r="F123" s="21"/>
+      <c r="G123" s="21"/>
+      <c r="H123" s="21"/>
+      <c r="I123" s="21"/>
+      <c r="J123" s="21"/>
+      <c r="K123" s="21"/>
+      <c r="L123" s="21"/>
+      <c r="M123" s="21"/>
+      <c r="N123" s="21"/>
+      <c r="O123" s="21"/>
+    </row>
+    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A124" s="21"/>
+      <c r="B124" s="21"/>
+      <c r="C124" s="21"/>
+      <c r="D124" s="21"/>
+      <c r="E124" s="21"/>
+      <c r="F124" s="21"/>
+      <c r="G124" s="21"/>
+      <c r="H124" s="21"/>
+      <c r="I124" s="21"/>
+      <c r="J124" s="21"/>
+      <c r="K124" s="21"/>
+      <c r="L124" s="21"/>
+      <c r="M124" s="21"/>
+      <c r="N124" s="21"/>
+      <c r="O124" s="21"/>
+    </row>
+    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A125" s="21"/>
+      <c r="B125" s="21"/>
+      <c r="C125" s="21"/>
+      <c r="D125" s="21"/>
+      <c r="E125" s="21"/>
+      <c r="F125" s="21"/>
+      <c r="G125" s="21"/>
+      <c r="H125" s="21"/>
+      <c r="I125" s="21"/>
+      <c r="J125" s="21"/>
+      <c r="K125" s="21"/>
+      <c r="L125" s="21"/>
+      <c r="M125" s="21"/>
+      <c r="N125" s="21"/>
+      <c r="O125" s="21"/>
+    </row>
+    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A126" s="21"/>
+      <c r="B126" s="21"/>
+      <c r="C126" s="21"/>
+      <c r="D126" s="21"/>
+      <c r="E126" s="21"/>
+      <c r="F126" s="21"/>
+      <c r="G126" s="21"/>
+      <c r="H126" s="21"/>
+      <c r="I126" s="21"/>
+      <c r="J126" s="21"/>
+      <c r="K126" s="21"/>
+      <c r="L126" s="21"/>
+      <c r="M126" s="21"/>
+      <c r="N126" s="21"/>
+      <c r="O126" s="21"/>
+    </row>
+    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A127" s="21"/>
+      <c r="B127" s="21"/>
+      <c r="C127" s="21"/>
+      <c r="D127" s="21"/>
+      <c r="E127" s="21"/>
+      <c r="F127" s="21"/>
+      <c r="G127" s="21"/>
+      <c r="H127" s="21"/>
+      <c r="I127" s="21"/>
+      <c r="J127" s="21"/>
+      <c r="K127" s="21"/>
+      <c r="L127" s="21"/>
+      <c r="M127" s="21"/>
+      <c r="N127" s="21"/>
+      <c r="O127" s="21"/>
+    </row>
+    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A128" s="21"/>
+      <c r="B128" s="21"/>
+      <c r="C128" s="21"/>
+      <c r="D128" s="21"/>
+      <c r="E128" s="21"/>
+      <c r="F128" s="21"/>
+      <c r="G128" s="21"/>
+      <c r="H128" s="21"/>
+      <c r="I128" s="21"/>
+      <c r="J128" s="21"/>
+      <c r="K128" s="21"/>
+      <c r="L128" s="21"/>
+      <c r="M128" s="21"/>
+      <c r="N128" s="21"/>
+      <c r="O128" s="21"/>
+    </row>
+    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A129" s="21"/>
+      <c r="B129" s="21"/>
+      <c r="C129" s="21"/>
+      <c r="D129" s="21"/>
+      <c r="E129" s="21"/>
+      <c r="F129" s="21"/>
+      <c r="G129" s="21"/>
+      <c r="H129" s="21"/>
+      <c r="I129" s="21"/>
+      <c r="J129" s="21"/>
+      <c r="K129" s="21"/>
+      <c r="L129" s="21"/>
+      <c r="M129" s="21"/>
+      <c r="N129" s="21"/>
+      <c r="O129" s="21"/>
+    </row>
+    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A130" s="21"/>
+      <c r="B130" s="21"/>
+      <c r="C130" s="21"/>
+      <c r="D130" s="21"/>
+      <c r="E130" s="21"/>
+      <c r="F130" s="21"/>
+      <c r="G130" s="21"/>
+      <c r="H130" s="21"/>
+      <c r="I130" s="21"/>
+      <c r="J130" s="21"/>
+      <c r="K130" s="21"/>
+      <c r="L130" s="21"/>
+      <c r="M130" s="21"/>
+      <c r="N130" s="21"/>
+      <c r="O130" s="21"/>
+    </row>
+    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A131" s="21"/>
+      <c r="B131" s="21"/>
+      <c r="C131" s="21"/>
+      <c r="D131" s="21"/>
+      <c r="E131" s="21"/>
+      <c r="F131" s="21"/>
+      <c r="G131" s="21"/>
+      <c r="H131" s="21"/>
+      <c r="I131" s="21"/>
+      <c r="J131" s="21"/>
+      <c r="K131" s="21"/>
+      <c r="L131" s="21"/>
+      <c r="M131" s="21"/>
+      <c r="N131" s="21"/>
+      <c r="O131" s="21"/>
+    </row>
+    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A132" s="21"/>
+      <c r="B132" s="21"/>
+      <c r="C132" s="21"/>
+      <c r="D132" s="21"/>
+      <c r="E132" s="21"/>
+      <c r="F132" s="21"/>
+      <c r="G132" s="21"/>
+      <c r="H132" s="21"/>
+      <c r="I132" s="21"/>
+      <c r="J132" s="21"/>
+      <c r="K132" s="21"/>
+      <c r="L132" s="21"/>
+      <c r="M132" s="21"/>
+      <c r="N132" s="21"/>
+      <c r="O132" s="21"/>
+    </row>
+    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A133" s="21"/>
+      <c r="B133" s="21"/>
+      <c r="C133" s="21"/>
+      <c r="D133" s="21"/>
+      <c r="E133" s="21"/>
+      <c r="F133" s="21"/>
+      <c r="G133" s="21"/>
+      <c r="H133" s="21"/>
+      <c r="I133" s="21"/>
+      <c r="J133" s="21"/>
+      <c r="K133" s="21"/>
+      <c r="L133" s="21"/>
+      <c r="M133" s="21"/>
+      <c r="N133" s="21"/>
+      <c r="O133" s="21"/>
+    </row>
+    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A134" s="21"/>
+      <c r="B134" s="21"/>
+      <c r="C134" s="21"/>
+      <c r="D134" s="21"/>
+      <c r="E134" s="21"/>
+      <c r="F134" s="21"/>
+      <c r="G134" s="21"/>
+      <c r="H134" s="21"/>
+      <c r="I134" s="21"/>
+      <c r="J134" s="21"/>
+      <c r="K134" s="21"/>
+      <c r="L134" s="21"/>
+      <c r="M134" s="21"/>
+      <c r="N134" s="21"/>
+      <c r="O134" s="21"/>
+    </row>
+    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A135" s="21"/>
+      <c r="B135" s="21"/>
+      <c r="C135" s="21"/>
+      <c r="D135" s="21"/>
+      <c r="E135" s="21"/>
+      <c r="F135" s="21"/>
+      <c r="G135" s="21"/>
+      <c r="H135" s="21"/>
+      <c r="I135" s="21"/>
+      <c r="J135" s="21"/>
+      <c r="K135" s="21"/>
+      <c r="L135" s="21"/>
+      <c r="M135" s="21"/>
+      <c r="N135" s="21"/>
+      <c r="O135" s="21"/>
+    </row>
+    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A136" s="21"/>
+      <c r="B136" s="21"/>
+      <c r="C136" s="21"/>
+      <c r="D136" s="21"/>
+      <c r="E136" s="21"/>
+      <c r="F136" s="21"/>
+      <c r="G136" s="21"/>
+      <c r="H136" s="21"/>
+      <c r="I136" s="21"/>
+      <c r="J136" s="21"/>
+      <c r="K136" s="21"/>
+      <c r="L136" s="21"/>
+      <c r="M136" s="21"/>
+      <c r="N136" s="21"/>
+      <c r="O136" s="21"/>
+    </row>
+    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A137" s="21"/>
+      <c r="B137" s="21"/>
+      <c r="C137" s="21"/>
+      <c r="D137" s="21"/>
+      <c r="E137" s="21"/>
+      <c r="F137" s="21"/>
+      <c r="G137" s="21"/>
+      <c r="H137" s="21"/>
+      <c r="I137" s="21"/>
+      <c r="J137" s="21"/>
+      <c r="K137" s="21"/>
+      <c r="L137" s="21"/>
+      <c r="M137" s="21"/>
+      <c r="N137" s="21"/>
+      <c r="O137" s="21"/>
+    </row>
+    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A138" s="21"/>
+      <c r="B138" s="21"/>
+      <c r="C138" s="21"/>
+      <c r="D138" s="21"/>
+      <c r="E138" s="21"/>
+      <c r="F138" s="21"/>
+      <c r="G138" s="21"/>
+      <c r="H138" s="21"/>
+      <c r="I138" s="21"/>
+      <c r="J138" s="21"/>
+      <c r="K138" s="21"/>
+      <c r="L138" s="21"/>
+      <c r="M138" s="21"/>
+      <c r="N138" s="21"/>
+      <c r="O138" s="21"/>
+    </row>
+    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A139" s="21"/>
+      <c r="B139" s="21"/>
+      <c r="C139" s="21"/>
+      <c r="D139" s="21"/>
+      <c r="E139" s="21"/>
+      <c r="F139" s="21"/>
+      <c r="G139" s="21"/>
+      <c r="H139" s="21"/>
+      <c r="I139" s="21"/>
+      <c r="J139" s="21"/>
+      <c r="K139" s="21"/>
+      <c r="L139" s="21"/>
+      <c r="M139" s="21"/>
+      <c r="N139" s="21"/>
+      <c r="O139" s="21"/>
+    </row>
+    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A140" s="21"/>
+      <c r="B140" s="21"/>
+      <c r="C140" s="21"/>
+      <c r="D140" s="21"/>
+      <c r="E140" s="21"/>
+      <c r="F140" s="21"/>
+      <c r="G140" s="21"/>
+      <c r="H140" s="21"/>
+      <c r="I140" s="21"/>
+      <c r="J140" s="21"/>
+      <c r="K140" s="21"/>
+      <c r="L140" s="21"/>
+      <c r="M140" s="21"/>
+      <c r="N140" s="21"/>
+      <c r="O140" s="21"/>
+    </row>
+    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A141" s="21"/>
+      <c r="B141" s="21"/>
+      <c r="C141" s="21"/>
+      <c r="D141" s="21"/>
+      <c r="E141" s="21"/>
+      <c r="F141" s="21"/>
+      <c r="G141" s="21"/>
+      <c r="H141" s="21"/>
+      <c r="I141" s="21"/>
+      <c r="J141" s="21"/>
+      <c r="K141" s="21"/>
+      <c r="L141" s="21"/>
+      <c r="M141" s="21"/>
+      <c r="N141" s="21"/>
+      <c r="O141" s="21"/>
+    </row>
+    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A142" s="21"/>
+      <c r="B142" s="21"/>
+      <c r="C142" s="21"/>
+      <c r="D142" s="21"/>
+      <c r="E142" s="21"/>
+      <c r="F142" s="21"/>
+      <c r="G142" s="21"/>
+      <c r="H142" s="21"/>
+      <c r="I142" s="21"/>
+      <c r="J142" s="21"/>
+      <c r="K142" s="21"/>
+      <c r="L142" s="21"/>
+      <c r="M142" s="21"/>
+      <c r="N142" s="21"/>
+      <c r="O142" s="21"/>
+    </row>
+    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A143" s="21"/>
+      <c r="B143" s="21"/>
+      <c r="C143" s="21"/>
+      <c r="D143" s="21"/>
+      <c r="E143" s="21"/>
+      <c r="F143" s="21"/>
+      <c r="G143" s="21"/>
+      <c r="H143" s="21"/>
+      <c r="I143" s="21"/>
+      <c r="J143" s="21"/>
+      <c r="K143" s="21"/>
+      <c r="L143" s="21"/>
+      <c r="M143" s="21"/>
+      <c r="N143" s="21"/>
+      <c r="O143" s="21"/>
+    </row>
+    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A144" s="21"/>
+      <c r="B144" s="21"/>
+      <c r="C144" s="21"/>
+      <c r="D144" s="21"/>
+      <c r="E144" s="21"/>
+      <c r="F144" s="21"/>
+      <c r="G144" s="21"/>
+      <c r="H144" s="21"/>
+      <c r="I144" s="21"/>
+      <c r="J144" s="21"/>
+      <c r="K144" s="21"/>
+      <c r="L144" s="21"/>
+      <c r="M144" s="21"/>
+      <c r="N144" s="21"/>
+      <c r="O144" s="21"/>
+    </row>
+    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A145" s="21"/>
+      <c r="B145" s="21"/>
+      <c r="C145" s="21"/>
+      <c r="D145" s="21"/>
+      <c r="E145" s="21"/>
+      <c r="F145" s="21"/>
+      <c r="G145" s="21"/>
+      <c r="H145" s="21"/>
+      <c r="I145" s="21"/>
+      <c r="J145" s="21"/>
+      <c r="K145" s="21"/>
+      <c r="L145" s="21"/>
+      <c r="M145" s="21"/>
+      <c r="N145" s="21"/>
+      <c r="O145" s="21"/>
+    </row>
+    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A146" s="21"/>
+      <c r="B146" s="21"/>
+      <c r="C146" s="21"/>
+      <c r="D146" s="21"/>
+      <c r="E146" s="21"/>
+      <c r="F146" s="21"/>
+      <c r="G146" s="21"/>
+      <c r="H146" s="21"/>
+      <c r="I146" s="21"/>
+      <c r="J146" s="21"/>
+      <c r="K146" s="21"/>
+      <c r="L146" s="21"/>
+      <c r="M146" s="21"/>
+      <c r="N146" s="21"/>
+      <c r="O146" s="21"/>
+    </row>
+    <row r="147" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A147" s="21"/>
+      <c r="B147" s="21"/>
+      <c r="C147" s="21"/>
+      <c r="D147" s="21"/>
+      <c r="E147" s="21"/>
+      <c r="F147" s="21"/>
+      <c r="G147" s="21"/>
+      <c r="H147" s="21"/>
+      <c r="I147" s="21"/>
+      <c r="J147" s="21"/>
+      <c r="K147" s="21"/>
+      <c r="L147" s="21"/>
+      <c r="M147" s="21"/>
+      <c r="N147" s="21"/>
+      <c r="O147" s="21"/>
+    </row>
+    <row r="148" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A148" s="21"/>
+      <c r="B148" s="21"/>
+      <c r="C148" s="21"/>
+      <c r="D148" s="21"/>
+      <c r="E148" s="21"/>
+      <c r="F148" s="21"/>
+      <c r="G148" s="21"/>
+      <c r="H148" s="21"/>
+      <c r="I148" s="21"/>
+      <c r="J148" s="21"/>
+      <c r="K148" s="21"/>
+      <c r="L148" s="21"/>
+      <c r="M148" s="21"/>
+      <c r="N148" s="21"/>
+      <c r="O148" s="21"/>
+    </row>
+    <row r="149" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A149" s="21"/>
+      <c r="B149" s="21"/>
+      <c r="C149" s="21"/>
+      <c r="D149" s="21"/>
+      <c r="E149" s="21"/>
+      <c r="F149" s="21"/>
+      <c r="G149" s="21"/>
+      <c r="H149" s="21"/>
+      <c r="I149" s="21"/>
+      <c r="J149" s="21"/>
+      <c r="K149" s="21"/>
+      <c r="L149" s="21"/>
+      <c r="M149" s="21"/>
+      <c r="N149" s="21"/>
+      <c r="O149" s="21"/>
+    </row>
+    <row r="150" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A150" s="21"/>
+      <c r="B150" s="21"/>
+      <c r="C150" s="21"/>
+      <c r="D150" s="21"/>
+      <c r="E150" s="21"/>
+      <c r="F150" s="21"/>
+      <c r="G150" s="21"/>
+      <c r="H150" s="21"/>
+      <c r="I150" s="21"/>
+      <c r="J150" s="21"/>
+      <c r="K150" s="21"/>
+      <c r="L150" s="21"/>
+      <c r="M150" s="21"/>
+      <c r="N150" s="21"/>
+      <c r="O150" s="21"/>
+    </row>
+    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A151" s="21"/>
+      <c r="B151" s="21"/>
+      <c r="C151" s="21"/>
+      <c r="D151" s="21"/>
+      <c r="E151" s="21"/>
+      <c r="F151" s="21"/>
+      <c r="G151" s="21"/>
+      <c r="H151" s="21"/>
+      <c r="I151" s="21"/>
+      <c r="J151" s="21"/>
+      <c r="K151" s="21"/>
+      <c r="L151" s="21"/>
+      <c r="M151" s="21"/>
+      <c r="N151" s="21"/>
+      <c r="O151" s="21"/>
+    </row>
+    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A152" s="21"/>
+      <c r="B152" s="21"/>
+      <c r="C152" s="21"/>
+      <c r="D152" s="21"/>
+      <c r="E152" s="21"/>
+      <c r="F152" s="21"/>
+      <c r="G152" s="21"/>
+      <c r="H152" s="21"/>
+      <c r="I152" s="21"/>
+      <c r="J152" s="21"/>
+      <c r="K152" s="21"/>
+      <c r="L152" s="21"/>
+      <c r="M152" s="21"/>
+      <c r="N152" s="21"/>
+      <c r="O152" s="21"/>
+    </row>
+    <row r="153" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A153" s="21"/>
+      <c r="B153" s="21"/>
+      <c r="C153" s="21"/>
+      <c r="D153" s="21"/>
+      <c r="E153" s="21"/>
+      <c r="F153" s="21"/>
+      <c r="G153" s="21"/>
+      <c r="H153" s="21"/>
+      <c r="I153" s="21"/>
+      <c r="J153" s="21"/>
+      <c r="K153" s="21"/>
+      <c r="L153" s="21"/>
+      <c r="M153" s="21"/>
+      <c r="N153" s="21"/>
+      <c r="O153" s="21"/>
+    </row>
+    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A154" s="21"/>
+      <c r="B154" s="21"/>
+      <c r="C154" s="21"/>
+      <c r="D154" s="21"/>
+      <c r="E154" s="21"/>
+      <c r="F154" s="21"/>
+      <c r="G154" s="21"/>
+      <c r="H154" s="21"/>
+      <c r="I154" s="21"/>
+      <c r="J154" s="21"/>
+      <c r="K154" s="21"/>
+      <c r="L154" s="21"/>
+      <c r="M154" s="21"/>
+      <c r="N154" s="21"/>
+      <c r="O154" s="21"/>
+    </row>
+    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A155" s="21"/>
+      <c r="B155" s="21"/>
+      <c r="C155" s="21"/>
+      <c r="D155" s="21"/>
+      <c r="E155" s="21"/>
+      <c r="F155" s="21"/>
+      <c r="G155" s="21"/>
+      <c r="H155" s="21"/>
+      <c r="I155" s="21"/>
+      <c r="J155" s="21"/>
+      <c r="K155" s="21"/>
+      <c r="L155" s="21"/>
+      <c r="M155" s="21"/>
+      <c r="N155" s="21"/>
+      <c r="O155" s="21"/>
+    </row>
+    <row r="156" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A156" s="21"/>
+      <c r="B156" s="21"/>
+      <c r="C156" s="21"/>
+      <c r="D156" s="21"/>
+      <c r="E156" s="21"/>
+      <c r="F156" s="21"/>
+      <c r="G156" s="21"/>
+      <c r="H156" s="21"/>
+      <c r="I156" s="21"/>
+      <c r="J156" s="21"/>
+      <c r="K156" s="21"/>
+      <c r="L156" s="21"/>
+      <c r="M156" s="21"/>
+      <c r="N156" s="21"/>
+      <c r="O156" s="21"/>
+    </row>
+    <row r="157" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A157" s="21"/>
+      <c r="B157" s="21"/>
+      <c r="C157" s="21"/>
+      <c r="D157" s="21"/>
+      <c r="E157" s="21"/>
+      <c r="F157" s="21"/>
+      <c r="G157" s="21"/>
+      <c r="H157" s="21"/>
+      <c r="I157" s="21"/>
+      <c r="J157" s="21"/>
+      <c r="K157" s="21"/>
+      <c r="L157" s="21"/>
+      <c r="M157" s="21"/>
+      <c r="N157" s="21"/>
+      <c r="O157" s="21"/>
+    </row>
+    <row r="158" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A158" s="21"/>
+      <c r="B158" s="21"/>
+      <c r="C158" s="21"/>
+      <c r="D158" s="21"/>
+      <c r="E158" s="21"/>
+      <c r="F158" s="21"/>
+      <c r="G158" s="21"/>
+      <c r="H158" s="21"/>
+      <c r="I158" s="21"/>
+      <c r="J158" s="21"/>
+      <c r="K158" s="21"/>
+      <c r="L158" s="21"/>
+      <c r="M158" s="21"/>
+      <c r="N158" s="21"/>
+      <c r="O158" s="21"/>
+    </row>
+    <row r="159" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A159" s="21"/>
+      <c r="B159" s="21"/>
+      <c r="C159" s="21"/>
+      <c r="D159" s="21"/>
+      <c r="E159" s="21"/>
+      <c r="F159" s="21"/>
+      <c r="G159" s="21"/>
+      <c r="H159" s="21"/>
+      <c r="I159" s="21"/>
+      <c r="J159" s="21"/>
+      <c r="K159" s="21"/>
+      <c r="L159" s="21"/>
+      <c r="M159" s="21"/>
+      <c r="N159" s="21"/>
+      <c r="O159" s="21"/>
+    </row>
+    <row r="160" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A160" s="21"/>
+      <c r="B160" s="21"/>
+      <c r="C160" s="21"/>
+      <c r="D160" s="21"/>
+      <c r="E160" s="21"/>
+      <c r="F160" s="21"/>
+      <c r="G160" s="21"/>
+      <c r="H160" s="21"/>
+      <c r="I160" s="21"/>
+      <c r="J160" s="21"/>
+      <c r="K160" s="21"/>
+      <c r="L160" s="21"/>
+      <c r="M160" s="21"/>
+      <c r="N160" s="21"/>
+      <c r="O160" s="21"/>
+    </row>
+    <row r="161" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A161" s="21"/>
+      <c r="B161" s="21"/>
+      <c r="C161" s="21"/>
+      <c r="D161" s="21"/>
+      <c r="E161" s="21"/>
+      <c r="F161" s="21"/>
+      <c r="G161" s="21"/>
+      <c r="H161" s="21"/>
+      <c r="I161" s="21"/>
+      <c r="J161" s="21"/>
+      <c r="K161" s="21"/>
+      <c r="L161" s="21"/>
+      <c r="M161" s="21"/>
+      <c r="N161" s="21"/>
+      <c r="O161" s="21"/>
+    </row>
+    <row r="162" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A162" s="21"/>
+      <c r="B162" s="21"/>
+      <c r="C162" s="21"/>
+      <c r="D162" s="21"/>
+      <c r="E162" s="21"/>
+      <c r="F162" s="21"/>
+      <c r="G162" s="21"/>
+      <c r="H162" s="21"/>
+      <c r="I162" s="21"/>
+      <c r="J162" s="21"/>
+      <c r="K162" s="21"/>
+      <c r="L162" s="21"/>
+      <c r="M162" s="21"/>
+      <c r="N162" s="21"/>
+      <c r="O162" s="21"/>
+    </row>
+    <row r="163" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A163" s="21"/>
+      <c r="B163" s="21"/>
+      <c r="C163" s="21"/>
+      <c r="D163" s="21"/>
+      <c r="E163" s="21"/>
+      <c r="F163" s="21"/>
+      <c r="G163" s="21"/>
+      <c r="H163" s="21"/>
+      <c r="I163" s="21"/>
+      <c r="J163" s="21"/>
+      <c r="K163" s="21"/>
+      <c r="L163" s="21"/>
+      <c r="M163" s="21"/>
+      <c r="N163" s="21"/>
+      <c r="O163" s="21"/>
+    </row>
+    <row r="164" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A164" s="21"/>
+      <c r="B164" s="21"/>
+      <c r="C164" s="21"/>
+      <c r="D164" s="21"/>
+      <c r="E164" s="21"/>
+      <c r="F164" s="21"/>
+      <c r="G164" s="21"/>
+      <c r="H164" s="21"/>
+      <c r="I164" s="21"/>
+      <c r="J164" s="21"/>
+      <c r="K164" s="21"/>
+      <c r="L164" s="21"/>
+      <c r="M164" s="21"/>
+      <c r="N164" s="21"/>
+      <c r="O164" s="21"/>
+    </row>
+    <row r="165" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A165" s="21"/>
+      <c r="B165" s="21"/>
+      <c r="C165" s="21"/>
+      <c r="D165" s="21"/>
+      <c r="E165" s="21"/>
+      <c r="F165" s="21"/>
+      <c r="G165" s="21"/>
+      <c r="H165" s="21"/>
+      <c r="I165" s="21"/>
+      <c r="J165" s="21"/>
+      <c r="K165" s="21"/>
+      <c r="L165" s="21"/>
+      <c r="M165" s="21"/>
+      <c r="N165" s="21"/>
+      <c r="O165" s="21"/>
+    </row>
+    <row r="166" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A166" s="21"/>
+      <c r="B166" s="21"/>
+      <c r="C166" s="21"/>
+      <c r="D166" s="21"/>
+      <c r="E166" s="21"/>
+      <c r="F166" s="21"/>
+      <c r="G166" s="21"/>
+      <c r="H166" s="21"/>
+      <c r="I166" s="21"/>
+      <c r="J166" s="21"/>
+      <c r="K166" s="21"/>
+      <c r="L166" s="21"/>
+      <c r="M166" s="21"/>
+      <c r="N166" s="21"/>
+      <c r="O166" s="21"/>
+    </row>
+    <row r="167" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A167" s="21"/>
+      <c r="B167" s="21"/>
+      <c r="C167" s="21"/>
+      <c r="D167" s="21"/>
+      <c r="E167" s="21"/>
+      <c r="F167" s="21"/>
+      <c r="G167" s="21"/>
+      <c r="H167" s="21"/>
+      <c r="I167" s="21"/>
+      <c r="J167" s="21"/>
+      <c r="K167" s="21"/>
+      <c r="L167" s="21"/>
+      <c r="M167" s="21"/>
+      <c r="N167" s="21"/>
+      <c r="O167" s="21"/>
+    </row>
+    <row r="168" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A168" s="21"/>
+      <c r="B168" s="21"/>
+      <c r="C168" s="21"/>
+      <c r="D168" s="21"/>
+      <c r="E168" s="21"/>
+      <c r="F168" s="21"/>
+      <c r="G168" s="21"/>
+      <c r="H168" s="21"/>
+      <c r="I168" s="21"/>
+      <c r="J168" s="21"/>
+      <c r="K168" s="21"/>
+      <c r="L168" s="21"/>
+      <c r="M168" s="21"/>
+      <c r="N168" s="21"/>
+      <c r="O168" s="21"/>
+    </row>
+    <row r="169" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A169" s="21"/>
+      <c r="B169" s="21"/>
+      <c r="C169" s="21"/>
+      <c r="D169" s="21"/>
+      <c r="E169" s="21"/>
+      <c r="F169" s="21"/>
+      <c r="G169" s="21"/>
+      <c r="H169" s="21"/>
+      <c r="I169" s="21"/>
+      <c r="J169" s="21"/>
+      <c r="K169" s="21"/>
+      <c r="L169" s="21"/>
+      <c r="M169" s="21"/>
+      <c r="N169" s="21"/>
+      <c r="O169" s="21"/>
+    </row>
+    <row r="170" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A170" s="21"/>
+      <c r="B170" s="21"/>
+      <c r="C170" s="21"/>
+      <c r="D170" s="21"/>
+      <c r="E170" s="21"/>
+      <c r="F170" s="21"/>
+      <c r="G170" s="21"/>
+      <c r="H170" s="21"/>
+      <c r="I170" s="21"/>
+      <c r="J170" s="21"/>
+      <c r="K170" s="21"/>
+      <c r="L170" s="21"/>
+      <c r="M170" s="21"/>
+      <c r="N170" s="21"/>
+      <c r="O170" s="21"/>
+    </row>
+    <row r="171" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A171" s="21"/>
+      <c r="B171" s="21"/>
+      <c r="C171" s="21"/>
+      <c r="D171" s="21"/>
+      <c r="E171" s="21"/>
+      <c r="F171" s="21"/>
+      <c r="G171" s="21"/>
+      <c r="H171" s="21"/>
+      <c r="I171" s="21"/>
+      <c r="J171" s="21"/>
+      <c r="K171" s="21"/>
+      <c r="L171" s="21"/>
+      <c r="M171" s="21"/>
+      <c r="N171" s="21"/>
+      <c r="O171" s="21"/>
+    </row>
+    <row r="172" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A172" s="21"/>
+      <c r="B172" s="21"/>
+      <c r="C172" s="21"/>
+      <c r="D172" s="21"/>
+      <c r="E172" s="21"/>
+      <c r="F172" s="21"/>
+      <c r="G172" s="21"/>
+      <c r="H172" s="21"/>
+      <c r="I172" s="21"/>
+      <c r="J172" s="21"/>
+      <c r="K172" s="21"/>
+      <c r="L172" s="21"/>
+      <c r="M172" s="21"/>
+      <c r="N172" s="21"/>
+      <c r="O172" s="21"/>
+    </row>
+    <row r="173" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A173" s="21"/>
+      <c r="B173" s="21"/>
+      <c r="C173" s="21"/>
+      <c r="D173" s="21"/>
+      <c r="E173" s="21"/>
+      <c r="F173" s="21"/>
+      <c r="G173" s="21"/>
+      <c r="H173" s="21"/>
+      <c r="I173" s="21"/>
+      <c r="J173" s="21"/>
+      <c r="K173" s="21"/>
+      <c r="L173" s="21"/>
+      <c r="M173" s="21"/>
+      <c r="N173" s="21"/>
+      <c r="O173" s="21"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I3" r:id="rId2"/>
+    <hyperlink ref="I5" r:id="rId3"/>
+    <hyperlink ref="I6" r:id="rId4"/>
+    <hyperlink ref="I24" r:id="rId5"/>
+    <hyperlink ref="I19" r:id="rId6"/>
+    <hyperlink ref="I11" r:id="rId7"/>
+    <hyperlink ref="I13" r:id="rId8"/>
+    <hyperlink ref="I18" r:id="rId9"/>
+    <hyperlink ref="I14" r:id="rId10"/>
+    <hyperlink ref="I17" r:id="rId11"/>
+    <hyperlink ref="I16" r:id="rId12"/>
+    <hyperlink ref="I15" r:id="rId13"/>
+    <hyperlink ref="I20" r:id="rId14"/>
+    <hyperlink ref="I12" r:id="rId15"/>
+    <hyperlink ref="I9" r:id="rId16"/>
+    <hyperlink ref="I4" r:id="rId17"/>
+    <hyperlink ref="I10" r:id="rId18"/>
+    <hyperlink ref="I23" r:id="rId19"/>
+    <hyperlink ref="I22" r:id="rId20"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId21"/>
+  <ignoredErrors>
+    <ignoredError sqref="D13:D17 D10:D11" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>